<commit_message>
Added functionality to test if rate transposing/detransposing works. It does.
</commit_message>
<xml_diff>
--- a/Primates/Mappe1 (Gemt automatisk).xlsx
+++ b/Primates/Mappe1 (Gemt automatisk).xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="21360" windowHeight="9240"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21360" windowHeight="9240"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
+    <sheet name="Ark2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="35">
   <si>
     <t>Primate 120:</t>
   </si>
@@ -100,12 +100,45 @@
   </si>
   <si>
     <t xml:space="preserve"> = index 47 =  first element of key</t>
+  </si>
+  <si>
+    <t>11111100 00000000 00000000 00000000 00000000 00000000 00000000</t>
+  </si>
+  <si>
+    <t>Dvs. Index 0 I strengen havner på index 55.</t>
+  </si>
+  <si>
+    <t>Efter transpose funktionen bliver brugt til at få en string med 6xFF, 0x00, 12xFF ind I raten på YMM:</t>
+  </si>
+  <si>
+    <t>Byte 0</t>
+  </si>
+  <si>
+    <t>Byte 1</t>
+  </si>
+  <si>
+    <t>Byte 2</t>
+  </si>
+  <si>
+    <t>Byte 3</t>
+  </si>
+  <si>
+    <t>Byte 4</t>
+  </si>
+  <si>
+    <t>Byte 5</t>
+  </si>
+  <si>
+    <t>Byte 6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="####"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -189,7 +222,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -200,6 +233,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -517,7 +551,7 @@
   <dimension ref="A1:CA28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AF8" sqref="AF8"/>
+      <selection activeCell="W6" sqref="W6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1404,6 +1438,78 @@
       <c r="CA5">
         <v>6</v>
       </c>
+    </row>
+    <row r="6" spans="1:79" x14ac:dyDescent="0.25">
+      <c r="X6" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y6" s="10"/>
+      <c r="Z6" s="10"/>
+      <c r="AA6" s="10"/>
+      <c r="AB6" s="10"/>
+      <c r="AC6" s="10"/>
+      <c r="AD6" s="10"/>
+      <c r="AE6" s="10"/>
+      <c r="AF6" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG6" s="10"/>
+      <c r="AH6" s="10"/>
+      <c r="AI6" s="10"/>
+      <c r="AJ6" s="10"/>
+      <c r="AK6" s="10"/>
+      <c r="AL6" s="10"/>
+      <c r="AM6" s="10"/>
+      <c r="AN6" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="AO6" s="10"/>
+      <c r="AP6" s="10"/>
+      <c r="AQ6" s="10"/>
+      <c r="AR6" s="10"/>
+      <c r="AS6" s="10"/>
+      <c r="AT6" s="10"/>
+      <c r="AU6" s="10"/>
+      <c r="AV6" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AW6" s="10"/>
+      <c r="AX6" s="10"/>
+      <c r="AY6" s="10"/>
+      <c r="AZ6" s="10"/>
+      <c r="BA6" s="10"/>
+      <c r="BB6" s="10"/>
+      <c r="BC6" s="10"/>
+      <c r="BD6" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="BE6" s="10"/>
+      <c r="BF6" s="10"/>
+      <c r="BG6" s="10"/>
+      <c r="BH6" s="10"/>
+      <c r="BI6" s="10"/>
+      <c r="BJ6" s="10"/>
+      <c r="BK6" s="10"/>
+      <c r="BL6" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="BM6" s="10"/>
+      <c r="BN6" s="10"/>
+      <c r="BO6" s="10"/>
+      <c r="BP6" s="10"/>
+      <c r="BQ6" s="10"/>
+      <c r="BR6" s="10"/>
+      <c r="BS6" s="10"/>
+      <c r="BT6" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="BU6" s="10"/>
+      <c r="BV6" s="10"/>
+      <c r="BW6" s="10"/>
+      <c r="BX6" s="10"/>
+      <c r="BY6" s="10"/>
+      <c r="BZ6" s="10"/>
+      <c r="CA6" s="10"/>
     </row>
     <row r="8" spans="1:79" x14ac:dyDescent="0.25">
       <c r="AF8" t="s">
@@ -1597,7 +1703,66 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="X6:AE6"/>
+    <mergeCell ref="BT6:CA6"/>
+    <mergeCell ref="BL6:BS6"/>
+    <mergeCell ref="BD6:BK6"/>
+    <mergeCell ref="AV6:BC6"/>
+    <mergeCell ref="AN6:AU6"/>
+    <mergeCell ref="AF6:AM6"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A8:A15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Example of me bufferoverflowing myself at line 689
</commit_message>
<xml_diff>
--- a/Primates/Mappe1 (Gemt automatisk).xlsx
+++ b/Primates/Mappe1 (Gemt automatisk).xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="94">
   <si>
     <t>Primate 120:</t>
   </si>
@@ -130,6 +130,183 @@
   </si>
   <si>
     <t>Byte 6</t>
+  </si>
+  <si>
+    <t>Old way</t>
+  </si>
+  <si>
+    <t>New way</t>
+  </si>
+  <si>
+    <t>r[row][col]</t>
+  </si>
+  <si>
+    <t>r7</t>
+  </si>
+  <si>
+    <t>c0</t>
+  </si>
+  <si>
+    <t>c1</t>
+  </si>
+  <si>
+    <t>c2</t>
+  </si>
+  <si>
+    <t>c3</t>
+  </si>
+  <si>
+    <t>c4</t>
+  </si>
+  <si>
+    <t>c5</t>
+  </si>
+  <si>
+    <t>c6</t>
+  </si>
+  <si>
+    <t>c7</t>
+  </si>
+  <si>
+    <t>c8</t>
+  </si>
+  <si>
+    <t>c16</t>
+  </si>
+  <si>
+    <t>c24</t>
+  </si>
+  <si>
+    <t>c21</t>
+  </si>
+  <si>
+    <t>c32</t>
+  </si>
+  <si>
+    <t>c40</t>
+  </si>
+  <si>
+    <t>c9</t>
+  </si>
+  <si>
+    <t>c10</t>
+  </si>
+  <si>
+    <t>c11</t>
+  </si>
+  <si>
+    <t>c12</t>
+  </si>
+  <si>
+    <t>c13</t>
+  </si>
+  <si>
+    <t>c14</t>
+  </si>
+  <si>
+    <t>c15</t>
+  </si>
+  <si>
+    <t>c17</t>
+  </si>
+  <si>
+    <t>c18</t>
+  </si>
+  <si>
+    <t>c19</t>
+  </si>
+  <si>
+    <t>c20</t>
+  </si>
+  <si>
+    <t>c22</t>
+  </si>
+  <si>
+    <t>c23</t>
+  </si>
+  <si>
+    <t>c25</t>
+  </si>
+  <si>
+    <t>c26</t>
+  </si>
+  <si>
+    <t>c27</t>
+  </si>
+  <si>
+    <t>c28</t>
+  </si>
+  <si>
+    <t>c29</t>
+  </si>
+  <si>
+    <t>c30</t>
+  </si>
+  <si>
+    <t>c31</t>
+  </si>
+  <si>
+    <t>c33</t>
+  </si>
+  <si>
+    <t>c34</t>
+  </si>
+  <si>
+    <t>c35</t>
+  </si>
+  <si>
+    <t>c36</t>
+  </si>
+  <si>
+    <t>c37</t>
+  </si>
+  <si>
+    <t>c38</t>
+  </si>
+  <si>
+    <t>c39</t>
+  </si>
+  <si>
+    <t>c41</t>
+  </si>
+  <si>
+    <t>c42</t>
+  </si>
+  <si>
+    <t>c43</t>
+  </si>
+  <si>
+    <t>c44</t>
+  </si>
+  <si>
+    <t>c45</t>
+  </si>
+  <si>
+    <t>c46</t>
+  </si>
+  <si>
+    <t>c47</t>
+  </si>
+  <si>
+    <t>1 left</t>
+  </si>
+  <si>
+    <t>2 left</t>
+  </si>
+  <si>
+    <t>3 left</t>
+  </si>
+  <si>
+    <t>4 left</t>
+  </si>
+  <si>
+    <t>0 left</t>
+  </si>
+  <si>
+    <t>5 left</t>
+  </si>
+  <si>
+    <t>7 left</t>
   </si>
 </sst>
 </file>
@@ -137,7 +314,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="####"/>
+    <numFmt numFmtId="164" formatCode="####"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -148,7 +325,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -209,6 +386,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -222,7 +405,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -233,7 +416,31 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -548,10 +755,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CA28"/>
+  <dimension ref="A1:CA57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="W6" sqref="W6"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J41" sqref="J41:Q41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -754,6 +961,9 @@
       </c>
     </row>
     <row r="2" spans="1:79" x14ac:dyDescent="0.25">
+      <c r="L2" t="s">
+        <v>35</v>
+      </c>
       <c r="X2" s="9" t="s">
         <v>8</v>
       </c>
@@ -1702,8 +1912,923 @@
         <v>23</v>
       </c>
     </row>
+    <row r="31" spans="1:79" x14ac:dyDescent="0.25">
+      <c r="J31" t="s">
+        <v>11</v>
+      </c>
+      <c r="K31" t="s">
+        <v>12</v>
+      </c>
+      <c r="L31" t="s">
+        <v>13</v>
+      </c>
+      <c r="M31" t="s">
+        <v>14</v>
+      </c>
+      <c r="N31" t="s">
+        <v>15</v>
+      </c>
+      <c r="O31" t="s">
+        <v>16</v>
+      </c>
+      <c r="P31" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>38</v>
+      </c>
+      <c r="S31" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="32" spans="1:79" x14ac:dyDescent="0.25">
+      <c r="J32" t="s">
+        <v>39</v>
+      </c>
+      <c r="K32" t="s">
+        <v>40</v>
+      </c>
+      <c r="L32" t="s">
+        <v>41</v>
+      </c>
+      <c r="M32" t="s">
+        <v>42</v>
+      </c>
+      <c r="N32" t="s">
+        <v>43</v>
+      </c>
+      <c r="O32" t="s">
+        <v>44</v>
+      </c>
+      <c r="P32" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>46</v>
+      </c>
+      <c r="S32" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="J33" t="s">
+        <v>47</v>
+      </c>
+      <c r="K33" t="s">
+        <v>53</v>
+      </c>
+      <c r="L33" t="s">
+        <v>54</v>
+      </c>
+      <c r="M33" t="s">
+        <v>55</v>
+      </c>
+      <c r="N33" t="s">
+        <v>56</v>
+      </c>
+      <c r="O33" t="s">
+        <v>57</v>
+      </c>
+      <c r="P33" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>59</v>
+      </c>
+      <c r="S33" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="34" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="J34" t="s">
+        <v>48</v>
+      </c>
+      <c r="K34" t="s">
+        <v>60</v>
+      </c>
+      <c r="L34" t="s">
+        <v>61</v>
+      </c>
+      <c r="M34" t="s">
+        <v>62</v>
+      </c>
+      <c r="N34" t="s">
+        <v>63</v>
+      </c>
+      <c r="O34" t="s">
+        <v>50</v>
+      </c>
+      <c r="P34" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>65</v>
+      </c>
+      <c r="S34" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="35" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="J35" t="s">
+        <v>49</v>
+      </c>
+      <c r="K35" t="s">
+        <v>66</v>
+      </c>
+      <c r="L35" t="s">
+        <v>67</v>
+      </c>
+      <c r="M35" t="s">
+        <v>68</v>
+      </c>
+      <c r="N35" t="s">
+        <v>69</v>
+      </c>
+      <c r="O35" t="s">
+        <v>70</v>
+      </c>
+      <c r="P35" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>72</v>
+      </c>
+      <c r="S35" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="36" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="J36" t="s">
+        <v>51</v>
+      </c>
+      <c r="K36" t="s">
+        <v>73</v>
+      </c>
+      <c r="L36" t="s">
+        <v>74</v>
+      </c>
+      <c r="M36" t="s">
+        <v>75</v>
+      </c>
+      <c r="N36" t="s">
+        <v>76</v>
+      </c>
+      <c r="O36" t="s">
+        <v>77</v>
+      </c>
+      <c r="P36" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>79</v>
+      </c>
+      <c r="S36" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="37" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="J37" t="s">
+        <v>52</v>
+      </c>
+      <c r="K37" t="s">
+        <v>80</v>
+      </c>
+      <c r="L37" t="s">
+        <v>81</v>
+      </c>
+      <c r="M37" t="s">
+        <v>82</v>
+      </c>
+      <c r="N37" t="s">
+        <v>83</v>
+      </c>
+      <c r="O37" t="s">
+        <v>84</v>
+      </c>
+      <c r="P37" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>86</v>
+      </c>
+      <c r="S37" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="38" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>36</v>
+      </c>
+      <c r="D38" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="B41" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" s="11"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="11"/>
+      <c r="H41" s="11"/>
+      <c r="I41" s="11"/>
+      <c r="J41" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="K41" s="12"/>
+      <c r="L41" s="12"/>
+      <c r="M41" s="12"/>
+      <c r="N41" s="12"/>
+      <c r="O41" s="12"/>
+      <c r="P41" s="12"/>
+      <c r="Q41" s="12"/>
+      <c r="R41" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="S41" s="13"/>
+      <c r="T41" s="13"/>
+      <c r="U41" s="13"/>
+      <c r="V41" s="13"/>
+      <c r="W41" s="13"/>
+      <c r="X41" s="13"/>
+      <c r="Y41" s="13"/>
+      <c r="Z41" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA41" s="14"/>
+      <c r="AB41" s="14"/>
+      <c r="AC41" s="14"/>
+      <c r="AD41" s="14"/>
+      <c r="AE41" s="14"/>
+      <c r="AF41" s="14"/>
+      <c r="AG41" s="14"/>
+      <c r="AH41" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="AI41" s="15"/>
+      <c r="AJ41" s="15"/>
+      <c r="AK41" s="15"/>
+      <c r="AL41" s="15"/>
+      <c r="AM41" s="15"/>
+      <c r="AN41" s="15"/>
+      <c r="AO41" s="15"/>
+      <c r="AP41" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="AQ41" s="16"/>
+      <c r="AR41" s="16"/>
+      <c r="AS41" s="16"/>
+      <c r="AT41" s="16"/>
+      <c r="AU41" s="16"/>
+      <c r="AV41" s="16"/>
+      <c r="AW41" s="16"/>
+      <c r="AX41" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="AY41" s="17"/>
+      <c r="AZ41" s="17"/>
+      <c r="BA41" s="17"/>
+      <c r="BB41" s="17"/>
+      <c r="BC41" s="17"/>
+      <c r="BD41" s="17"/>
+      <c r="BE41" s="17"/>
+      <c r="BF41" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="BG41" s="18"/>
+      <c r="BH41" s="18"/>
+      <c r="BI41" s="18"/>
+      <c r="BJ41" s="18"/>
+      <c r="BK41" s="18"/>
+      <c r="BL41" s="18"/>
+      <c r="BM41" s="18"/>
+    </row>
+    <row r="43" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="B43" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
+      <c r="E43" s="11"/>
+      <c r="F43" s="11"/>
+      <c r="G43" s="11"/>
+      <c r="H43" s="11"/>
+      <c r="I43" s="11"/>
+      <c r="J43" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="K43" s="12"/>
+      <c r="L43" s="12"/>
+      <c r="M43" s="12"/>
+      <c r="N43" s="12"/>
+      <c r="O43" s="12"/>
+      <c r="P43" s="12"/>
+      <c r="Q43" s="12"/>
+      <c r="R43" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="S43" s="13"/>
+      <c r="T43" s="13"/>
+      <c r="U43" s="13"/>
+      <c r="V43" s="13"/>
+      <c r="W43" s="13"/>
+      <c r="X43" s="13"/>
+      <c r="Y43" s="13"/>
+      <c r="Z43" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA43" s="14"/>
+      <c r="AB43" s="14"/>
+      <c r="AC43" s="14"/>
+      <c r="AD43" s="14"/>
+      <c r="AE43" s="14"/>
+      <c r="AF43" s="14"/>
+      <c r="AG43" s="14"/>
+      <c r="AH43" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="AI43" s="15"/>
+      <c r="AJ43" s="15"/>
+      <c r="AK43" s="15"/>
+      <c r="AL43" s="15"/>
+      <c r="AM43" s="15"/>
+      <c r="AN43" s="15"/>
+      <c r="AO43" s="15"/>
+      <c r="AP43" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="AQ43" s="16"/>
+      <c r="AR43" s="16"/>
+      <c r="AS43" s="16"/>
+      <c r="AT43" s="16"/>
+      <c r="AU43" s="16"/>
+      <c r="AV43" s="16"/>
+      <c r="AW43" s="16"/>
+      <c r="AX43" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="AY43" s="17"/>
+      <c r="AZ43" s="17"/>
+      <c r="BA43" s="17"/>
+      <c r="BB43" s="17"/>
+      <c r="BC43" s="17"/>
+      <c r="BD43" s="17"/>
+      <c r="BE43" s="17"/>
+      <c r="BF43" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="BG43" s="18"/>
+      <c r="BH43" s="18"/>
+      <c r="BI43" s="18"/>
+      <c r="BJ43" s="18"/>
+      <c r="BK43" s="18"/>
+      <c r="BL43" s="18"/>
+      <c r="BM43" s="18"/>
+    </row>
+    <row r="45" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="B45" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C45" s="11"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="11"/>
+      <c r="G45" s="11"/>
+      <c r="H45" s="11"/>
+      <c r="I45" s="11"/>
+      <c r="J45" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="K45" s="12"/>
+      <c r="L45" s="12"/>
+      <c r="M45" s="12"/>
+      <c r="N45" s="12"/>
+      <c r="O45" s="12"/>
+      <c r="P45" s="12"/>
+      <c r="Q45" s="12"/>
+      <c r="R45" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="S45" s="13"/>
+      <c r="T45" s="13"/>
+      <c r="U45" s="13"/>
+      <c r="V45" s="13"/>
+      <c r="W45" s="13"/>
+      <c r="X45" s="13"/>
+      <c r="Y45" s="13"/>
+      <c r="Z45" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA45" s="14"/>
+      <c r="AB45" s="14"/>
+      <c r="AC45" s="14"/>
+      <c r="AD45" s="14"/>
+      <c r="AE45" s="14"/>
+      <c r="AF45" s="14"/>
+      <c r="AG45" s="14"/>
+      <c r="AH45" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI45" s="15"/>
+      <c r="AJ45" s="15"/>
+      <c r="AK45" s="15"/>
+      <c r="AL45" s="15"/>
+      <c r="AM45" s="15"/>
+      <c r="AN45" s="15"/>
+      <c r="AO45" s="15"/>
+      <c r="AP45" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="AQ45" s="16"/>
+      <c r="AR45" s="16"/>
+      <c r="AS45" s="16"/>
+      <c r="AT45" s="16"/>
+      <c r="AU45" s="16"/>
+      <c r="AV45" s="16"/>
+      <c r="AW45" s="16"/>
+      <c r="AX45" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="AY45" s="17"/>
+      <c r="AZ45" s="17"/>
+      <c r="BA45" s="17"/>
+      <c r="BB45" s="17"/>
+      <c r="BC45" s="17"/>
+      <c r="BD45" s="17"/>
+      <c r="BE45" s="17"/>
+      <c r="BF45" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="BG45" s="18"/>
+      <c r="BH45" s="18"/>
+      <c r="BI45" s="18"/>
+      <c r="BJ45" s="18"/>
+      <c r="BK45" s="18"/>
+      <c r="BL45" s="18"/>
+      <c r="BM45" s="18"/>
+    </row>
+    <row r="47" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="B47" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C47" s="11"/>
+      <c r="D47" s="11"/>
+      <c r="E47" s="11"/>
+      <c r="F47" s="11"/>
+      <c r="G47" s="11"/>
+      <c r="H47" s="11"/>
+      <c r="I47" s="11"/>
+      <c r="J47" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="K47" s="12"/>
+      <c r="L47" s="12"/>
+      <c r="M47" s="12"/>
+      <c r="N47" s="12"/>
+      <c r="O47" s="12"/>
+      <c r="P47" s="12"/>
+      <c r="Q47" s="12"/>
+      <c r="R47" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="S47" s="13"/>
+      <c r="T47" s="13"/>
+      <c r="U47" s="13"/>
+      <c r="V47" s="13"/>
+      <c r="W47" s="13"/>
+      <c r="X47" s="13"/>
+      <c r="Y47" s="13"/>
+      <c r="Z47" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA47" s="14"/>
+      <c r="AB47" s="14"/>
+      <c r="AC47" s="14"/>
+      <c r="AD47" s="14"/>
+      <c r="AE47" s="14"/>
+      <c r="AF47" s="14"/>
+      <c r="AG47" s="14"/>
+      <c r="AH47" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="AI47" s="15"/>
+      <c r="AJ47" s="15"/>
+      <c r="AK47" s="15"/>
+      <c r="AL47" s="15"/>
+      <c r="AM47" s="15"/>
+      <c r="AN47" s="15"/>
+      <c r="AO47" s="15"/>
+      <c r="AP47" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="AQ47" s="16"/>
+      <c r="AR47" s="16"/>
+      <c r="AS47" s="16"/>
+      <c r="AT47" s="16"/>
+      <c r="AU47" s="16"/>
+      <c r="AV47" s="16"/>
+      <c r="AW47" s="16"/>
+      <c r="AX47" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="AY47" s="17"/>
+      <c r="AZ47" s="17"/>
+      <c r="BA47" s="17"/>
+      <c r="BB47" s="17"/>
+      <c r="BC47" s="17"/>
+      <c r="BD47" s="17"/>
+      <c r="BE47" s="17"/>
+      <c r="BF47" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="BG47" s="18"/>
+      <c r="BH47" s="18"/>
+      <c r="BI47" s="18"/>
+      <c r="BJ47" s="18"/>
+      <c r="BK47" s="18"/>
+      <c r="BL47" s="18"/>
+      <c r="BM47" s="18"/>
+    </row>
+    <row r="51" spans="2:65" x14ac:dyDescent="0.25">
+      <c r="B51" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C51" s="11"/>
+      <c r="D51" s="11"/>
+      <c r="E51" s="11"/>
+      <c r="F51" s="11"/>
+      <c r="G51" s="11"/>
+      <c r="H51" s="11"/>
+      <c r="I51" s="11"/>
+      <c r="J51" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="K51" s="12"/>
+      <c r="L51" s="12"/>
+      <c r="M51" s="12"/>
+      <c r="N51" s="12"/>
+      <c r="O51" s="12"/>
+      <c r="P51" s="12"/>
+      <c r="Q51" s="12"/>
+      <c r="R51" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="S51" s="13"/>
+      <c r="T51" s="13"/>
+      <c r="U51" s="13"/>
+      <c r="V51" s="13"/>
+      <c r="W51" s="13"/>
+      <c r="X51" s="13"/>
+      <c r="Y51" s="13"/>
+      <c r="Z51" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA51" s="14"/>
+      <c r="AB51" s="14"/>
+      <c r="AC51" s="14"/>
+      <c r="AD51" s="14"/>
+      <c r="AE51" s="14"/>
+      <c r="AF51" s="14"/>
+      <c r="AG51" s="14"/>
+      <c r="AH51" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="AI51" s="15"/>
+      <c r="AJ51" s="15"/>
+      <c r="AK51" s="15"/>
+      <c r="AL51" s="15"/>
+      <c r="AM51" s="15"/>
+      <c r="AN51" s="15"/>
+      <c r="AO51" s="15"/>
+      <c r="AP51" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AQ51" s="16"/>
+      <c r="AR51" s="16"/>
+      <c r="AS51" s="16"/>
+      <c r="AT51" s="16"/>
+      <c r="AU51" s="16"/>
+      <c r="AV51" s="16"/>
+      <c r="AW51" s="16"/>
+      <c r="AX51" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="AY51" s="17"/>
+      <c r="AZ51" s="17"/>
+      <c r="BA51" s="17"/>
+      <c r="BB51" s="17"/>
+      <c r="BC51" s="17"/>
+      <c r="BD51" s="17"/>
+      <c r="BE51" s="17"/>
+      <c r="BF51" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="BG51" s="18"/>
+      <c r="BH51" s="18"/>
+      <c r="BI51" s="18"/>
+      <c r="BJ51" s="18"/>
+      <c r="BK51" s="18"/>
+      <c r="BL51" s="18"/>
+      <c r="BM51" s="18"/>
+    </row>
+    <row r="53" spans="2:65" x14ac:dyDescent="0.25">
+      <c r="B53" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C53" s="11"/>
+      <c r="D53" s="11"/>
+      <c r="E53" s="11"/>
+      <c r="F53" s="11"/>
+      <c r="G53" s="11"/>
+      <c r="H53" s="11"/>
+      <c r="I53" s="11"/>
+      <c r="J53" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="K53" s="12"/>
+      <c r="L53" s="12"/>
+      <c r="M53" s="12"/>
+      <c r="N53" s="12"/>
+      <c r="O53" s="12"/>
+      <c r="P53" s="12"/>
+      <c r="Q53" s="12"/>
+      <c r="R53" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="S53" s="13"/>
+      <c r="T53" s="13"/>
+      <c r="U53" s="13"/>
+      <c r="V53" s="13"/>
+      <c r="W53" s="13"/>
+      <c r="X53" s="13"/>
+      <c r="Y53" s="13"/>
+      <c r="Z53" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA53" s="14"/>
+      <c r="AB53" s="14"/>
+      <c r="AC53" s="14"/>
+      <c r="AD53" s="14"/>
+      <c r="AE53" s="14"/>
+      <c r="AF53" s="14"/>
+      <c r="AG53" s="14"/>
+      <c r="AH53" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="AI53" s="15"/>
+      <c r="AJ53" s="15"/>
+      <c r="AK53" s="15"/>
+      <c r="AL53" s="15"/>
+      <c r="AM53" s="15"/>
+      <c r="AN53" s="15"/>
+      <c r="AO53" s="15"/>
+      <c r="AP53" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="AQ53" s="16"/>
+      <c r="AR53" s="16"/>
+      <c r="AS53" s="16"/>
+      <c r="AT53" s="16"/>
+      <c r="AU53" s="16"/>
+      <c r="AV53" s="16"/>
+      <c r="AW53" s="16"/>
+      <c r="AX53" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="AY53" s="17"/>
+      <c r="AZ53" s="17"/>
+      <c r="BA53" s="17"/>
+      <c r="BB53" s="17"/>
+      <c r="BC53" s="17"/>
+      <c r="BD53" s="17"/>
+      <c r="BE53" s="17"/>
+      <c r="BF53" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="BG53" s="18"/>
+      <c r="BH53" s="18"/>
+      <c r="BI53" s="18"/>
+      <c r="BJ53" s="18"/>
+      <c r="BK53" s="18"/>
+      <c r="BL53" s="18"/>
+      <c r="BM53" s="18"/>
+    </row>
+    <row r="55" spans="2:65" x14ac:dyDescent="0.25">
+      <c r="B55" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C55" s="11"/>
+      <c r="D55" s="11"/>
+      <c r="E55" s="11"/>
+      <c r="F55" s="11"/>
+      <c r="G55" s="11"/>
+      <c r="H55" s="11"/>
+      <c r="I55" s="11"/>
+      <c r="J55" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="K55" s="12"/>
+      <c r="L55" s="12"/>
+      <c r="M55" s="12"/>
+      <c r="N55" s="12"/>
+      <c r="O55" s="12"/>
+      <c r="P55" s="12"/>
+      <c r="Q55" s="12"/>
+      <c r="R55" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="S55" s="13"/>
+      <c r="T55" s="13"/>
+      <c r="U55" s="13"/>
+      <c r="V55" s="13"/>
+      <c r="W55" s="13"/>
+      <c r="X55" s="13"/>
+      <c r="Y55" s="13"/>
+      <c r="Z55" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA55" s="14"/>
+      <c r="AB55" s="14"/>
+      <c r="AC55" s="14"/>
+      <c r="AD55" s="14"/>
+      <c r="AE55" s="14"/>
+      <c r="AF55" s="14"/>
+      <c r="AG55" s="14"/>
+      <c r="AH55" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="AI55" s="15"/>
+      <c r="AJ55" s="15"/>
+      <c r="AK55" s="15"/>
+      <c r="AL55" s="15"/>
+      <c r="AM55" s="15"/>
+      <c r="AN55" s="15"/>
+      <c r="AO55" s="15"/>
+      <c r="AP55" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="AQ55" s="16"/>
+      <c r="AR55" s="16"/>
+      <c r="AS55" s="16"/>
+      <c r="AT55" s="16"/>
+      <c r="AU55" s="16"/>
+      <c r="AV55" s="16"/>
+      <c r="AW55" s="16"/>
+      <c r="AX55" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="AY55" s="17"/>
+      <c r="AZ55" s="17"/>
+      <c r="BA55" s="17"/>
+      <c r="BB55" s="17"/>
+      <c r="BC55" s="17"/>
+      <c r="BD55" s="17"/>
+      <c r="BE55" s="17"/>
+      <c r="BF55" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="BG55" s="18"/>
+      <c r="BH55" s="18"/>
+      <c r="BI55" s="18"/>
+      <c r="BJ55" s="18"/>
+      <c r="BK55" s="18"/>
+      <c r="BL55" s="18"/>
+      <c r="BM55" s="18"/>
+    </row>
+    <row r="57" spans="2:65" x14ac:dyDescent="0.25">
+      <c r="B57" s="11"/>
+      <c r="C57" s="11"/>
+      <c r="D57" s="11"/>
+      <c r="E57" s="11"/>
+      <c r="F57" s="11"/>
+      <c r="G57" s="11"/>
+      <c r="H57" s="11"/>
+      <c r="I57" s="11"/>
+      <c r="J57" s="12"/>
+      <c r="K57" s="12"/>
+      <c r="L57" s="12"/>
+      <c r="M57" s="12"/>
+      <c r="N57" s="12"/>
+      <c r="O57" s="12"/>
+      <c r="P57" s="12"/>
+      <c r="Q57" s="12"/>
+      <c r="R57" s="13"/>
+      <c r="S57" s="13"/>
+      <c r="T57" s="13"/>
+      <c r="U57" s="13"/>
+      <c r="V57" s="13"/>
+      <c r="W57" s="13"/>
+      <c r="X57" s="13"/>
+      <c r="Y57" s="13"/>
+      <c r="Z57" s="14"/>
+      <c r="AA57" s="14"/>
+      <c r="AB57" s="14"/>
+      <c r="AC57" s="14"/>
+      <c r="AD57" s="14"/>
+      <c r="AE57" s="14"/>
+      <c r="AF57" s="14"/>
+      <c r="AG57" s="14"/>
+      <c r="AH57" s="15"/>
+      <c r="AI57" s="15"/>
+      <c r="AJ57" s="15"/>
+      <c r="AK57" s="15"/>
+      <c r="AL57" s="15"/>
+      <c r="AM57" s="15"/>
+      <c r="AN57" s="15"/>
+      <c r="AO57" s="15"/>
+      <c r="AP57" s="16"/>
+      <c r="AQ57" s="16"/>
+      <c r="AR57" s="16"/>
+      <c r="AS57" s="16"/>
+      <c r="AT57" s="16"/>
+      <c r="AU57" s="16"/>
+      <c r="AV57" s="16"/>
+      <c r="AW57" s="16"/>
+      <c r="AX57" s="17"/>
+      <c r="AY57" s="17"/>
+      <c r="AZ57" s="17"/>
+      <c r="BA57" s="17"/>
+      <c r="BB57" s="17"/>
+      <c r="BC57" s="17"/>
+      <c r="BD57" s="17"/>
+      <c r="BE57" s="17"/>
+      <c r="BF57" s="18"/>
+      <c r="BG57" s="18"/>
+      <c r="BH57" s="18"/>
+      <c r="BI57" s="18"/>
+      <c r="BJ57" s="18"/>
+      <c r="BK57" s="18"/>
+      <c r="BL57" s="18"/>
+      <c r="BM57" s="18"/>
+    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="71">
+    <mergeCell ref="BF47:BM47"/>
+    <mergeCell ref="BF51:BM51"/>
+    <mergeCell ref="BF53:BM53"/>
+    <mergeCell ref="BF55:BM55"/>
+    <mergeCell ref="BF57:BM57"/>
+    <mergeCell ref="AX45:BE45"/>
+    <mergeCell ref="AX43:BE43"/>
+    <mergeCell ref="AX41:BE41"/>
+    <mergeCell ref="BF41:BM41"/>
+    <mergeCell ref="BF43:BM43"/>
+    <mergeCell ref="BF45:BM45"/>
+    <mergeCell ref="AX57:BE57"/>
+    <mergeCell ref="AX55:BE55"/>
+    <mergeCell ref="AX53:BE53"/>
+    <mergeCell ref="AX51:BE51"/>
+    <mergeCell ref="AX47:BE47"/>
+    <mergeCell ref="AH53:AO53"/>
+    <mergeCell ref="AH55:AO55"/>
+    <mergeCell ref="AH57:AO57"/>
+    <mergeCell ref="AP41:AW41"/>
+    <mergeCell ref="AP43:AW43"/>
+    <mergeCell ref="AP45:AW45"/>
+    <mergeCell ref="AP47:AW47"/>
+    <mergeCell ref="AP51:AW51"/>
+    <mergeCell ref="AP53:AW53"/>
+    <mergeCell ref="AP55:AW55"/>
+    <mergeCell ref="AP57:AW57"/>
+    <mergeCell ref="AH41:AO41"/>
+    <mergeCell ref="AH43:AO43"/>
+    <mergeCell ref="AH45:AO45"/>
+    <mergeCell ref="AH47:AO47"/>
+    <mergeCell ref="AH51:AO51"/>
+    <mergeCell ref="R53:Y53"/>
+    <mergeCell ref="R55:Y55"/>
+    <mergeCell ref="R57:Y57"/>
+    <mergeCell ref="Z41:AG41"/>
+    <mergeCell ref="Z43:AG43"/>
+    <mergeCell ref="Z45:AG45"/>
+    <mergeCell ref="Z47:AG47"/>
+    <mergeCell ref="Z51:AG51"/>
+    <mergeCell ref="Z53:AG53"/>
+    <mergeCell ref="Z55:AG55"/>
+    <mergeCell ref="Z57:AG57"/>
+    <mergeCell ref="R41:Y41"/>
+    <mergeCell ref="R43:Y43"/>
+    <mergeCell ref="R45:Y45"/>
+    <mergeCell ref="R47:Y47"/>
+    <mergeCell ref="R51:Y51"/>
+    <mergeCell ref="J51:Q51"/>
+    <mergeCell ref="J53:Q53"/>
+    <mergeCell ref="J55:Q55"/>
+    <mergeCell ref="J57:Q57"/>
+    <mergeCell ref="B43:I43"/>
+    <mergeCell ref="B45:I45"/>
+    <mergeCell ref="B47:I47"/>
+    <mergeCell ref="B51:I51"/>
+    <mergeCell ref="B53:I53"/>
+    <mergeCell ref="B55:I55"/>
+    <mergeCell ref="B57:I57"/>
+    <mergeCell ref="B41:I41"/>
+    <mergeCell ref="J43:Q43"/>
+    <mergeCell ref="J41:Q41"/>
+    <mergeCell ref="J45:Q45"/>
+    <mergeCell ref="J47:Q47"/>
     <mergeCell ref="X6:AE6"/>
     <mergeCell ref="BT6:CA6"/>
     <mergeCell ref="BL6:BS6"/>

</xml_diff>

<commit_message>
Shiftrows + inv implemented for primate 120. Subbytes + inv implemented. MixCol + constant addition missing
</commit_message>
<xml_diff>
--- a/Primates/Mappe1 (Gemt automatisk).xlsx
+++ b/Primates/Mappe1 (Gemt automatisk).xlsx
@@ -416,11 +416,16 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -429,18 +434,13 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -758,7 +758,7 @@
   <dimension ref="A1:CA57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A24" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J41" sqref="J41:Q41"/>
+      <selection activeCell="BB54" sqref="BB54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1650,76 +1650,76 @@
       </c>
     </row>
     <row r="6" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="X6" s="10" t="s">
+      <c r="X6" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="Y6" s="10"/>
-      <c r="Z6" s="10"/>
-      <c r="AA6" s="10"/>
-      <c r="AB6" s="10"/>
-      <c r="AC6" s="10"/>
-      <c r="AD6" s="10"/>
-      <c r="AE6" s="10"/>
-      <c r="AF6" s="10" t="s">
+      <c r="Y6" s="18"/>
+      <c r="Z6" s="18"/>
+      <c r="AA6" s="18"/>
+      <c r="AB6" s="18"/>
+      <c r="AC6" s="18"/>
+      <c r="AD6" s="18"/>
+      <c r="AE6" s="18"/>
+      <c r="AF6" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="AG6" s="10"/>
-      <c r="AH6" s="10"/>
-      <c r="AI6" s="10"/>
-      <c r="AJ6" s="10"/>
-      <c r="AK6" s="10"/>
-      <c r="AL6" s="10"/>
-      <c r="AM6" s="10"/>
-      <c r="AN6" s="10" t="s">
+      <c r="AG6" s="18"/>
+      <c r="AH6" s="18"/>
+      <c r="AI6" s="18"/>
+      <c r="AJ6" s="18"/>
+      <c r="AK6" s="18"/>
+      <c r="AL6" s="18"/>
+      <c r="AM6" s="18"/>
+      <c r="AN6" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="AO6" s="10"/>
-      <c r="AP6" s="10"/>
-      <c r="AQ6" s="10"/>
-      <c r="AR6" s="10"/>
-      <c r="AS6" s="10"/>
-      <c r="AT6" s="10"/>
-      <c r="AU6" s="10"/>
-      <c r="AV6" s="10" t="s">
+      <c r="AO6" s="18"/>
+      <c r="AP6" s="18"/>
+      <c r="AQ6" s="18"/>
+      <c r="AR6" s="18"/>
+      <c r="AS6" s="18"/>
+      <c r="AT6" s="18"/>
+      <c r="AU6" s="18"/>
+      <c r="AV6" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="AW6" s="10"/>
-      <c r="AX6" s="10"/>
-      <c r="AY6" s="10"/>
-      <c r="AZ6" s="10"/>
-      <c r="BA6" s="10"/>
-      <c r="BB6" s="10"/>
-      <c r="BC6" s="10"/>
-      <c r="BD6" s="10" t="s">
+      <c r="AW6" s="18"/>
+      <c r="AX6" s="18"/>
+      <c r="AY6" s="18"/>
+      <c r="AZ6" s="18"/>
+      <c r="BA6" s="18"/>
+      <c r="BB6" s="18"/>
+      <c r="BC6" s="18"/>
+      <c r="BD6" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="BE6" s="10"/>
-      <c r="BF6" s="10"/>
-      <c r="BG6" s="10"/>
-      <c r="BH6" s="10"/>
-      <c r="BI6" s="10"/>
-      <c r="BJ6" s="10"/>
-      <c r="BK6" s="10"/>
-      <c r="BL6" s="10" t="s">
+      <c r="BE6" s="18"/>
+      <c r="BF6" s="18"/>
+      <c r="BG6" s="18"/>
+      <c r="BH6" s="18"/>
+      <c r="BI6" s="18"/>
+      <c r="BJ6" s="18"/>
+      <c r="BK6" s="18"/>
+      <c r="BL6" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="BM6" s="10"/>
-      <c r="BN6" s="10"/>
-      <c r="BO6" s="10"/>
-      <c r="BP6" s="10"/>
-      <c r="BQ6" s="10"/>
-      <c r="BR6" s="10"/>
-      <c r="BS6" s="10"/>
-      <c r="BT6" s="10" t="s">
+      <c r="BM6" s="18"/>
+      <c r="BN6" s="18"/>
+      <c r="BO6" s="18"/>
+      <c r="BP6" s="18"/>
+      <c r="BQ6" s="18"/>
+      <c r="BR6" s="18"/>
+      <c r="BS6" s="18"/>
+      <c r="BT6" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="BU6" s="10"/>
-      <c r="BV6" s="10"/>
-      <c r="BW6" s="10"/>
-      <c r="BX6" s="10"/>
-      <c r="BY6" s="10"/>
-      <c r="BZ6" s="10"/>
-      <c r="CA6" s="10"/>
+      <c r="BU6" s="18"/>
+      <c r="BV6" s="18"/>
+      <c r="BW6" s="18"/>
+      <c r="BX6" s="18"/>
+      <c r="BY6" s="18"/>
+      <c r="BZ6" s="18"/>
+      <c r="CA6" s="18"/>
     </row>
     <row r="8" spans="1:79" x14ac:dyDescent="0.25">
       <c r="AF8" t="s">
@@ -2124,663 +2124,764 @@
       </c>
     </row>
     <row r="41" spans="1:65" x14ac:dyDescent="0.25">
-      <c r="B41" s="11" t="s">
+      <c r="B41" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C41" s="11"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="11"/>
-      <c r="F41" s="11"/>
-      <c r="G41" s="11"/>
-      <c r="H41" s="11"/>
-      <c r="I41" s="11"/>
-      <c r="J41" s="12" t="s">
+      <c r="C41" s="17"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="17"/>
+      <c r="F41" s="17"/>
+      <c r="G41" s="17"/>
+      <c r="H41" s="17"/>
+      <c r="I41" s="17"/>
+      <c r="J41" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="K41" s="12"/>
-      <c r="L41" s="12"/>
-      <c r="M41" s="12"/>
-      <c r="N41" s="12"/>
-      <c r="O41" s="12"/>
-      <c r="P41" s="12"/>
-      <c r="Q41" s="12"/>
-      <c r="R41" s="13" t="s">
+      <c r="K41" s="16"/>
+      <c r="L41" s="16"/>
+      <c r="M41" s="16"/>
+      <c r="N41" s="16"/>
+      <c r="O41" s="16"/>
+      <c r="P41" s="16"/>
+      <c r="Q41" s="16"/>
+      <c r="R41" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="S41" s="13"/>
-      <c r="T41" s="13"/>
-      <c r="U41" s="13"/>
-      <c r="V41" s="13"/>
-      <c r="W41" s="13"/>
-      <c r="X41" s="13"/>
-      <c r="Y41" s="13"/>
-      <c r="Z41" s="14" t="s">
+      <c r="S41" s="14"/>
+      <c r="T41" s="14"/>
+      <c r="U41" s="14"/>
+      <c r="V41" s="14"/>
+      <c r="W41" s="14"/>
+      <c r="X41" s="14"/>
+      <c r="Y41" s="14"/>
+      <c r="Z41" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="AA41" s="14"/>
-      <c r="AB41" s="14"/>
-      <c r="AC41" s="14"/>
-      <c r="AD41" s="14"/>
-      <c r="AE41" s="14"/>
-      <c r="AF41" s="14"/>
-      <c r="AG41" s="14"/>
-      <c r="AH41" s="15" t="s">
+      <c r="AA41" s="15"/>
+      <c r="AB41" s="15"/>
+      <c r="AC41" s="15"/>
+      <c r="AD41" s="15"/>
+      <c r="AE41" s="15"/>
+      <c r="AF41" s="15"/>
+      <c r="AG41" s="15"/>
+      <c r="AH41" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="AI41" s="15"/>
-      <c r="AJ41" s="15"/>
-      <c r="AK41" s="15"/>
-      <c r="AL41" s="15"/>
-      <c r="AM41" s="15"/>
-      <c r="AN41" s="15"/>
-      <c r="AO41" s="15"/>
-      <c r="AP41" s="16" t="s">
+      <c r="AI41" s="12"/>
+      <c r="AJ41" s="12"/>
+      <c r="AK41" s="12"/>
+      <c r="AL41" s="12"/>
+      <c r="AM41" s="12"/>
+      <c r="AN41" s="12"/>
+      <c r="AO41" s="12"/>
+      <c r="AP41" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="AQ41" s="16"/>
-      <c r="AR41" s="16"/>
-      <c r="AS41" s="16"/>
-      <c r="AT41" s="16"/>
-      <c r="AU41" s="16"/>
-      <c r="AV41" s="16"/>
-      <c r="AW41" s="16"/>
-      <c r="AX41" s="17" t="s">
+      <c r="AQ41" s="13"/>
+      <c r="AR41" s="13"/>
+      <c r="AS41" s="13"/>
+      <c r="AT41" s="13"/>
+      <c r="AU41" s="13"/>
+      <c r="AV41" s="13"/>
+      <c r="AW41" s="13"/>
+      <c r="AX41" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="AY41" s="17"/>
-      <c r="AZ41" s="17"/>
-      <c r="BA41" s="17"/>
-      <c r="BB41" s="17"/>
-      <c r="BC41" s="17"/>
-      <c r="BD41" s="17"/>
-      <c r="BE41" s="17"/>
-      <c r="BF41" s="18" t="s">
+      <c r="AY41" s="11"/>
+      <c r="AZ41" s="11"/>
+      <c r="BA41" s="11"/>
+      <c r="BB41" s="11"/>
+      <c r="BC41" s="11"/>
+      <c r="BD41" s="11"/>
+      <c r="BE41" s="11"/>
+      <c r="BF41" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="BG41" s="18"/>
-      <c r="BH41" s="18"/>
-      <c r="BI41" s="18"/>
-      <c r="BJ41" s="18"/>
-      <c r="BK41" s="18"/>
-      <c r="BL41" s="18"/>
-      <c r="BM41" s="18"/>
+      <c r="BG41" s="10"/>
+      <c r="BH41" s="10"/>
+      <c r="BI41" s="10"/>
+      <c r="BJ41" s="10"/>
+      <c r="BK41" s="10"/>
+      <c r="BL41" s="10"/>
+      <c r="BM41" s="10"/>
     </row>
     <row r="43" spans="1:65" x14ac:dyDescent="0.25">
-      <c r="B43" s="11" t="s">
+      <c r="B43" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="C43" s="11"/>
-      <c r="D43" s="11"/>
-      <c r="E43" s="11"/>
-      <c r="F43" s="11"/>
-      <c r="G43" s="11"/>
-      <c r="H43" s="11"/>
-      <c r="I43" s="11"/>
-      <c r="J43" s="12" t="s">
+      <c r="C43" s="17"/>
+      <c r="D43" s="17"/>
+      <c r="E43" s="17"/>
+      <c r="F43" s="17"/>
+      <c r="G43" s="17"/>
+      <c r="H43" s="17"/>
+      <c r="I43" s="17"/>
+      <c r="J43" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="K43" s="12"/>
-      <c r="L43" s="12"/>
-      <c r="M43" s="12"/>
-      <c r="N43" s="12"/>
-      <c r="O43" s="12"/>
-      <c r="P43" s="12"/>
-      <c r="Q43" s="12"/>
-      <c r="R43" s="13" t="s">
+      <c r="K43" s="16"/>
+      <c r="L43" s="16"/>
+      <c r="M43" s="16"/>
+      <c r="N43" s="16"/>
+      <c r="O43" s="16"/>
+      <c r="P43" s="16"/>
+      <c r="Q43" s="16"/>
+      <c r="R43" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="S43" s="13"/>
-      <c r="T43" s="13"/>
-      <c r="U43" s="13"/>
-      <c r="V43" s="13"/>
-      <c r="W43" s="13"/>
-      <c r="X43" s="13"/>
-      <c r="Y43" s="13"/>
-      <c r="Z43" s="14" t="s">
+      <c r="S43" s="14"/>
+      <c r="T43" s="14"/>
+      <c r="U43" s="14"/>
+      <c r="V43" s="14"/>
+      <c r="W43" s="14"/>
+      <c r="X43" s="14"/>
+      <c r="Y43" s="14"/>
+      <c r="Z43" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="AA43" s="14"/>
-      <c r="AB43" s="14"/>
-      <c r="AC43" s="14"/>
-      <c r="AD43" s="14"/>
-      <c r="AE43" s="14"/>
-      <c r="AF43" s="14"/>
-      <c r="AG43" s="14"/>
-      <c r="AH43" s="15" t="s">
+      <c r="AA43" s="15"/>
+      <c r="AB43" s="15"/>
+      <c r="AC43" s="15"/>
+      <c r="AD43" s="15"/>
+      <c r="AE43" s="15"/>
+      <c r="AF43" s="15"/>
+      <c r="AG43" s="15"/>
+      <c r="AH43" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="AI43" s="15"/>
-      <c r="AJ43" s="15"/>
-      <c r="AK43" s="15"/>
-      <c r="AL43" s="15"/>
-      <c r="AM43" s="15"/>
-      <c r="AN43" s="15"/>
-      <c r="AO43" s="15"/>
-      <c r="AP43" s="16" t="s">
+      <c r="AI43" s="12"/>
+      <c r="AJ43" s="12"/>
+      <c r="AK43" s="12"/>
+      <c r="AL43" s="12"/>
+      <c r="AM43" s="12"/>
+      <c r="AN43" s="12"/>
+      <c r="AO43" s="12"/>
+      <c r="AP43" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="AQ43" s="16"/>
-      <c r="AR43" s="16"/>
-      <c r="AS43" s="16"/>
-      <c r="AT43" s="16"/>
-      <c r="AU43" s="16"/>
-      <c r="AV43" s="16"/>
-      <c r="AW43" s="16"/>
-      <c r="AX43" s="17" t="s">
+      <c r="AQ43" s="13"/>
+      <c r="AR43" s="13"/>
+      <c r="AS43" s="13"/>
+      <c r="AT43" s="13"/>
+      <c r="AU43" s="13"/>
+      <c r="AV43" s="13"/>
+      <c r="AW43" s="13"/>
+      <c r="AX43" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="AY43" s="17"/>
-      <c r="AZ43" s="17"/>
-      <c r="BA43" s="17"/>
-      <c r="BB43" s="17"/>
-      <c r="BC43" s="17"/>
-      <c r="BD43" s="17"/>
-      <c r="BE43" s="17"/>
-      <c r="BF43" s="18" t="s">
+      <c r="AY43" s="11"/>
+      <c r="AZ43" s="11"/>
+      <c r="BA43" s="11"/>
+      <c r="BB43" s="11"/>
+      <c r="BC43" s="11"/>
+      <c r="BD43" s="11"/>
+      <c r="BE43" s="11"/>
+      <c r="BF43" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="BG43" s="18"/>
-      <c r="BH43" s="18"/>
-      <c r="BI43" s="18"/>
-      <c r="BJ43" s="18"/>
-      <c r="BK43" s="18"/>
-      <c r="BL43" s="18"/>
-      <c r="BM43" s="18"/>
+      <c r="BG43" s="10"/>
+      <c r="BH43" s="10"/>
+      <c r="BI43" s="10"/>
+      <c r="BJ43" s="10"/>
+      <c r="BK43" s="10"/>
+      <c r="BL43" s="10"/>
+      <c r="BM43" s="10"/>
     </row>
     <row r="45" spans="1:65" x14ac:dyDescent="0.25">
-      <c r="B45" s="11" t="s">
+      <c r="B45" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="C45" s="11"/>
-      <c r="D45" s="11"/>
-      <c r="E45" s="11"/>
-      <c r="F45" s="11"/>
-      <c r="G45" s="11"/>
-      <c r="H45" s="11"/>
-      <c r="I45" s="11"/>
-      <c r="J45" s="12" t="s">
+      <c r="C45" s="17"/>
+      <c r="D45" s="17"/>
+      <c r="E45" s="17"/>
+      <c r="F45" s="17"/>
+      <c r="G45" s="17"/>
+      <c r="H45" s="17"/>
+      <c r="I45" s="17"/>
+      <c r="J45" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="K45" s="12"/>
-      <c r="L45" s="12"/>
-      <c r="M45" s="12"/>
-      <c r="N45" s="12"/>
-      <c r="O45" s="12"/>
-      <c r="P45" s="12"/>
-      <c r="Q45" s="12"/>
-      <c r="R45" s="13" t="s">
+      <c r="K45" s="16"/>
+      <c r="L45" s="16"/>
+      <c r="M45" s="16"/>
+      <c r="N45" s="16"/>
+      <c r="O45" s="16"/>
+      <c r="P45" s="16"/>
+      <c r="Q45" s="16"/>
+      <c r="R45" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="S45" s="13"/>
-      <c r="T45" s="13"/>
-      <c r="U45" s="13"/>
-      <c r="V45" s="13"/>
-      <c r="W45" s="13"/>
-      <c r="X45" s="13"/>
-      <c r="Y45" s="13"/>
-      <c r="Z45" s="14" t="s">
+      <c r="S45" s="14"/>
+      <c r="T45" s="14"/>
+      <c r="U45" s="14"/>
+      <c r="V45" s="14"/>
+      <c r="W45" s="14"/>
+      <c r="X45" s="14"/>
+      <c r="Y45" s="14"/>
+      <c r="Z45" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="AA45" s="14"/>
-      <c r="AB45" s="14"/>
-      <c r="AC45" s="14"/>
-      <c r="AD45" s="14"/>
-      <c r="AE45" s="14"/>
-      <c r="AF45" s="14"/>
-      <c r="AG45" s="14"/>
-      <c r="AH45" s="15" t="s">
+      <c r="AA45" s="15"/>
+      <c r="AB45" s="15"/>
+      <c r="AC45" s="15"/>
+      <c r="AD45" s="15"/>
+      <c r="AE45" s="15"/>
+      <c r="AF45" s="15"/>
+      <c r="AG45" s="15"/>
+      <c r="AH45" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="AI45" s="15"/>
-      <c r="AJ45" s="15"/>
-      <c r="AK45" s="15"/>
-      <c r="AL45" s="15"/>
-      <c r="AM45" s="15"/>
-      <c r="AN45" s="15"/>
-      <c r="AO45" s="15"/>
-      <c r="AP45" s="16" t="s">
+      <c r="AI45" s="12"/>
+      <c r="AJ45" s="12"/>
+      <c r="AK45" s="12"/>
+      <c r="AL45" s="12"/>
+      <c r="AM45" s="12"/>
+      <c r="AN45" s="12"/>
+      <c r="AO45" s="12"/>
+      <c r="AP45" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="AQ45" s="16"/>
-      <c r="AR45" s="16"/>
-      <c r="AS45" s="16"/>
-      <c r="AT45" s="16"/>
-      <c r="AU45" s="16"/>
-      <c r="AV45" s="16"/>
-      <c r="AW45" s="16"/>
-      <c r="AX45" s="17" t="s">
+      <c r="AQ45" s="13"/>
+      <c r="AR45" s="13"/>
+      <c r="AS45" s="13"/>
+      <c r="AT45" s="13"/>
+      <c r="AU45" s="13"/>
+      <c r="AV45" s="13"/>
+      <c r="AW45" s="13"/>
+      <c r="AX45" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="AY45" s="17"/>
-      <c r="AZ45" s="17"/>
-      <c r="BA45" s="17"/>
-      <c r="BB45" s="17"/>
-      <c r="BC45" s="17"/>
-      <c r="BD45" s="17"/>
-      <c r="BE45" s="17"/>
-      <c r="BF45" s="18" t="s">
+      <c r="AY45" s="11"/>
+      <c r="AZ45" s="11"/>
+      <c r="BA45" s="11"/>
+      <c r="BB45" s="11"/>
+      <c r="BC45" s="11"/>
+      <c r="BD45" s="11"/>
+      <c r="BE45" s="11"/>
+      <c r="BF45" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="BG45" s="18"/>
-      <c r="BH45" s="18"/>
-      <c r="BI45" s="18"/>
-      <c r="BJ45" s="18"/>
-      <c r="BK45" s="18"/>
-      <c r="BL45" s="18"/>
-      <c r="BM45" s="18"/>
+      <c r="BG45" s="10"/>
+      <c r="BH45" s="10"/>
+      <c r="BI45" s="10"/>
+      <c r="BJ45" s="10"/>
+      <c r="BK45" s="10"/>
+      <c r="BL45" s="10"/>
+      <c r="BM45" s="10"/>
     </row>
     <row r="47" spans="1:65" x14ac:dyDescent="0.25">
-      <c r="B47" s="11" t="s">
+      <c r="B47" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="C47" s="11"/>
-      <c r="D47" s="11"/>
-      <c r="E47" s="11"/>
-      <c r="F47" s="11"/>
-      <c r="G47" s="11"/>
-      <c r="H47" s="11"/>
-      <c r="I47" s="11"/>
-      <c r="J47" s="12" t="s">
+      <c r="C47" s="17"/>
+      <c r="D47" s="17"/>
+      <c r="E47" s="17"/>
+      <c r="F47" s="17"/>
+      <c r="G47" s="17"/>
+      <c r="H47" s="17"/>
+      <c r="I47" s="17"/>
+      <c r="J47" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="K47" s="12"/>
-      <c r="L47" s="12"/>
-      <c r="M47" s="12"/>
-      <c r="N47" s="12"/>
-      <c r="O47" s="12"/>
-      <c r="P47" s="12"/>
-      <c r="Q47" s="12"/>
-      <c r="R47" s="13" t="s">
+      <c r="K47" s="16"/>
+      <c r="L47" s="16"/>
+      <c r="M47" s="16"/>
+      <c r="N47" s="16"/>
+      <c r="O47" s="16"/>
+      <c r="P47" s="16"/>
+      <c r="Q47" s="16"/>
+      <c r="R47" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="S47" s="13"/>
-      <c r="T47" s="13"/>
-      <c r="U47" s="13"/>
-      <c r="V47" s="13"/>
-      <c r="W47" s="13"/>
-      <c r="X47" s="13"/>
-      <c r="Y47" s="13"/>
-      <c r="Z47" s="14" t="s">
+      <c r="S47" s="14"/>
+      <c r="T47" s="14"/>
+      <c r="U47" s="14"/>
+      <c r="V47" s="14"/>
+      <c r="W47" s="14"/>
+      <c r="X47" s="14"/>
+      <c r="Y47" s="14"/>
+      <c r="Z47" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="AA47" s="14"/>
-      <c r="AB47" s="14"/>
-      <c r="AC47" s="14"/>
-      <c r="AD47" s="14"/>
-      <c r="AE47" s="14"/>
-      <c r="AF47" s="14"/>
-      <c r="AG47" s="14"/>
-      <c r="AH47" s="15" t="s">
+      <c r="AA47" s="15"/>
+      <c r="AB47" s="15"/>
+      <c r="AC47" s="15"/>
+      <c r="AD47" s="15"/>
+      <c r="AE47" s="15"/>
+      <c r="AF47" s="15"/>
+      <c r="AG47" s="15"/>
+      <c r="AH47" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="AI47" s="15"/>
-      <c r="AJ47" s="15"/>
-      <c r="AK47" s="15"/>
-      <c r="AL47" s="15"/>
-      <c r="AM47" s="15"/>
-      <c r="AN47" s="15"/>
-      <c r="AO47" s="15"/>
-      <c r="AP47" s="16" t="s">
+      <c r="AI47" s="12"/>
+      <c r="AJ47" s="12"/>
+      <c r="AK47" s="12"/>
+      <c r="AL47" s="12"/>
+      <c r="AM47" s="12"/>
+      <c r="AN47" s="12"/>
+      <c r="AO47" s="12"/>
+      <c r="AP47" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="AQ47" s="16"/>
-      <c r="AR47" s="16"/>
-      <c r="AS47" s="16"/>
-      <c r="AT47" s="16"/>
-      <c r="AU47" s="16"/>
-      <c r="AV47" s="16"/>
-      <c r="AW47" s="16"/>
-      <c r="AX47" s="17" t="s">
+      <c r="AQ47" s="13"/>
+      <c r="AR47" s="13"/>
+      <c r="AS47" s="13"/>
+      <c r="AT47" s="13"/>
+      <c r="AU47" s="13"/>
+      <c r="AV47" s="13"/>
+      <c r="AW47" s="13"/>
+      <c r="AX47" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="AY47" s="17"/>
-      <c r="AZ47" s="17"/>
-      <c r="BA47" s="17"/>
-      <c r="BB47" s="17"/>
-      <c r="BC47" s="17"/>
-      <c r="BD47" s="17"/>
-      <c r="BE47" s="17"/>
-      <c r="BF47" s="18" t="s">
+      <c r="AY47" s="11"/>
+      <c r="AZ47" s="11"/>
+      <c r="BA47" s="11"/>
+      <c r="BB47" s="11"/>
+      <c r="BC47" s="11"/>
+      <c r="BD47" s="11"/>
+      <c r="BE47" s="11"/>
+      <c r="BF47" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="BG47" s="18"/>
-      <c r="BH47" s="18"/>
-      <c r="BI47" s="18"/>
-      <c r="BJ47" s="18"/>
-      <c r="BK47" s="18"/>
-      <c r="BL47" s="18"/>
-      <c r="BM47" s="18"/>
+      <c r="BG47" s="10"/>
+      <c r="BH47" s="10"/>
+      <c r="BI47" s="10"/>
+      <c r="BJ47" s="10"/>
+      <c r="BK47" s="10"/>
+      <c r="BL47" s="10"/>
+      <c r="BM47" s="10"/>
+    </row>
+    <row r="50" spans="2:65" x14ac:dyDescent="0.25">
+      <c r="B50">
+        <v>0</v>
+      </c>
+      <c r="J50">
+        <v>1</v>
+      </c>
+      <c r="R50">
+        <v>2</v>
+      </c>
+      <c r="Z50">
+        <v>3</v>
+      </c>
+      <c r="AH50">
+        <v>4</v>
+      </c>
+      <c r="AP50">
+        <v>5</v>
+      </c>
+      <c r="AX50">
+        <v>6</v>
+      </c>
+      <c r="BF50">
+        <v>7</v>
+      </c>
     </row>
     <row r="51" spans="2:65" x14ac:dyDescent="0.25">
-      <c r="B51" s="11" t="s">
+      <c r="B51" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="C51" s="11"/>
-      <c r="D51" s="11"/>
-      <c r="E51" s="11"/>
-      <c r="F51" s="11"/>
-      <c r="G51" s="11"/>
-      <c r="H51" s="11"/>
-      <c r="I51" s="11"/>
-      <c r="J51" s="12" t="s">
+      <c r="C51" s="17"/>
+      <c r="D51" s="17"/>
+      <c r="E51" s="17"/>
+      <c r="F51" s="17"/>
+      <c r="G51" s="17"/>
+      <c r="H51" s="17"/>
+      <c r="I51" s="17"/>
+      <c r="J51" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="K51" s="12"/>
-      <c r="L51" s="12"/>
-      <c r="M51" s="12"/>
-      <c r="N51" s="12"/>
-      <c r="O51" s="12"/>
-      <c r="P51" s="12"/>
-      <c r="Q51" s="12"/>
-      <c r="R51" s="13" t="s">
+      <c r="K51" s="16"/>
+      <c r="L51" s="16"/>
+      <c r="M51" s="16"/>
+      <c r="N51" s="16"/>
+      <c r="O51" s="16"/>
+      <c r="P51" s="16"/>
+      <c r="Q51" s="16"/>
+      <c r="R51" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="S51" s="13"/>
-      <c r="T51" s="13"/>
-      <c r="U51" s="13"/>
-      <c r="V51" s="13"/>
-      <c r="W51" s="13"/>
-      <c r="X51" s="13"/>
-      <c r="Y51" s="13"/>
-      <c r="Z51" s="14" t="s">
+      <c r="S51" s="14"/>
+      <c r="T51" s="14"/>
+      <c r="U51" s="14"/>
+      <c r="V51" s="14"/>
+      <c r="W51" s="14"/>
+      <c r="X51" s="14"/>
+      <c r="Y51" s="14"/>
+      <c r="Z51" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="AA51" s="14"/>
-      <c r="AB51" s="14"/>
-      <c r="AC51" s="14"/>
-      <c r="AD51" s="14"/>
-      <c r="AE51" s="14"/>
-      <c r="AF51" s="14"/>
-      <c r="AG51" s="14"/>
-      <c r="AH51" s="15" t="s">
+      <c r="AA51" s="15"/>
+      <c r="AB51" s="15"/>
+      <c r="AC51" s="15"/>
+      <c r="AD51" s="15"/>
+      <c r="AE51" s="15"/>
+      <c r="AF51" s="15"/>
+      <c r="AG51" s="15"/>
+      <c r="AH51" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="AI51" s="15"/>
-      <c r="AJ51" s="15"/>
-      <c r="AK51" s="15"/>
-      <c r="AL51" s="15"/>
-      <c r="AM51" s="15"/>
-      <c r="AN51" s="15"/>
-      <c r="AO51" s="15"/>
-      <c r="AP51" s="16" t="s">
+      <c r="AI51" s="12"/>
+      <c r="AJ51" s="12"/>
+      <c r="AK51" s="12"/>
+      <c r="AL51" s="12"/>
+      <c r="AM51" s="12"/>
+      <c r="AN51" s="12"/>
+      <c r="AO51" s="12"/>
+      <c r="AP51" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="AQ51" s="16"/>
-      <c r="AR51" s="16"/>
-      <c r="AS51" s="16"/>
-      <c r="AT51" s="16"/>
-      <c r="AU51" s="16"/>
-      <c r="AV51" s="16"/>
-      <c r="AW51" s="16"/>
-      <c r="AX51" s="17" t="s">
+      <c r="AQ51" s="13"/>
+      <c r="AR51" s="13"/>
+      <c r="AS51" s="13"/>
+      <c r="AT51" s="13"/>
+      <c r="AU51" s="13"/>
+      <c r="AV51" s="13"/>
+      <c r="AW51" s="13"/>
+      <c r="AX51" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="AY51" s="17"/>
-      <c r="AZ51" s="17"/>
-      <c r="BA51" s="17"/>
-      <c r="BB51" s="17"/>
-      <c r="BC51" s="17"/>
-      <c r="BD51" s="17"/>
-      <c r="BE51" s="17"/>
-      <c r="BF51" s="18" t="s">
+      <c r="AY51" s="11"/>
+      <c r="AZ51" s="11"/>
+      <c r="BA51" s="11"/>
+      <c r="BB51" s="11"/>
+      <c r="BC51" s="11"/>
+      <c r="BD51" s="11"/>
+      <c r="BE51" s="11"/>
+      <c r="BF51" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="BG51" s="18"/>
-      <c r="BH51" s="18"/>
-      <c r="BI51" s="18"/>
-      <c r="BJ51" s="18"/>
-      <c r="BK51" s="18"/>
-      <c r="BL51" s="18"/>
-      <c r="BM51" s="18"/>
+      <c r="BG51" s="10"/>
+      <c r="BH51" s="10"/>
+      <c r="BI51" s="10"/>
+      <c r="BJ51" s="10"/>
+      <c r="BK51" s="10"/>
+      <c r="BL51" s="10"/>
+      <c r="BM51" s="10"/>
+    </row>
+    <row r="52" spans="2:65" x14ac:dyDescent="0.25">
+      <c r="B52">
+        <v>8</v>
+      </c>
+      <c r="J52">
+        <v>9</v>
+      </c>
+      <c r="R52">
+        <v>10</v>
+      </c>
+      <c r="Z52">
+        <v>11</v>
+      </c>
+      <c r="AH52">
+        <v>12</v>
+      </c>
+      <c r="AP52">
+        <v>13</v>
+      </c>
+      <c r="AX52">
+        <v>14</v>
+      </c>
+      <c r="BF52">
+        <v>15</v>
+      </c>
     </row>
     <row r="53" spans="2:65" x14ac:dyDescent="0.25">
-      <c r="B53" s="11" t="s">
+      <c r="B53" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="C53" s="11"/>
-      <c r="D53" s="11"/>
-      <c r="E53" s="11"/>
-      <c r="F53" s="11"/>
-      <c r="G53" s="11"/>
-      <c r="H53" s="11"/>
-      <c r="I53" s="11"/>
-      <c r="J53" s="12" t="s">
+      <c r="C53" s="17"/>
+      <c r="D53" s="17"/>
+      <c r="E53" s="17"/>
+      <c r="F53" s="17"/>
+      <c r="G53" s="17"/>
+      <c r="H53" s="17"/>
+      <c r="I53" s="17"/>
+      <c r="J53" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="K53" s="12"/>
-      <c r="L53" s="12"/>
-      <c r="M53" s="12"/>
-      <c r="N53" s="12"/>
-      <c r="O53" s="12"/>
-      <c r="P53" s="12"/>
-      <c r="Q53" s="12"/>
-      <c r="R53" s="13" t="s">
+      <c r="K53" s="16"/>
+      <c r="L53" s="16"/>
+      <c r="M53" s="16"/>
+      <c r="N53" s="16"/>
+      <c r="O53" s="16"/>
+      <c r="P53" s="16"/>
+      <c r="Q53" s="16"/>
+      <c r="R53" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="S53" s="13"/>
-      <c r="T53" s="13"/>
-      <c r="U53" s="13"/>
-      <c r="V53" s="13"/>
-      <c r="W53" s="13"/>
-      <c r="X53" s="13"/>
-      <c r="Y53" s="13"/>
-      <c r="Z53" s="14" t="s">
+      <c r="S53" s="14"/>
+      <c r="T53" s="14"/>
+      <c r="U53" s="14"/>
+      <c r="V53" s="14"/>
+      <c r="W53" s="14"/>
+      <c r="X53" s="14"/>
+      <c r="Y53" s="14"/>
+      <c r="Z53" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="AA53" s="14"/>
-      <c r="AB53" s="14"/>
-      <c r="AC53" s="14"/>
-      <c r="AD53" s="14"/>
-      <c r="AE53" s="14"/>
-      <c r="AF53" s="14"/>
-      <c r="AG53" s="14"/>
-      <c r="AH53" s="15" t="s">
+      <c r="AA53" s="15"/>
+      <c r="AB53" s="15"/>
+      <c r="AC53" s="15"/>
+      <c r="AD53" s="15"/>
+      <c r="AE53" s="15"/>
+      <c r="AF53" s="15"/>
+      <c r="AG53" s="15"/>
+      <c r="AH53" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="AI53" s="15"/>
-      <c r="AJ53" s="15"/>
-      <c r="AK53" s="15"/>
-      <c r="AL53" s="15"/>
-      <c r="AM53" s="15"/>
-      <c r="AN53" s="15"/>
-      <c r="AO53" s="15"/>
-      <c r="AP53" s="16" t="s">
+      <c r="AI53" s="12"/>
+      <c r="AJ53" s="12"/>
+      <c r="AK53" s="12"/>
+      <c r="AL53" s="12"/>
+      <c r="AM53" s="12"/>
+      <c r="AN53" s="12"/>
+      <c r="AO53" s="12"/>
+      <c r="AP53" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="AQ53" s="16"/>
-      <c r="AR53" s="16"/>
-      <c r="AS53" s="16"/>
-      <c r="AT53" s="16"/>
-      <c r="AU53" s="16"/>
-      <c r="AV53" s="16"/>
-      <c r="AW53" s="16"/>
-      <c r="AX53" s="17" t="s">
+      <c r="AQ53" s="13"/>
+      <c r="AR53" s="13"/>
+      <c r="AS53" s="13"/>
+      <c r="AT53" s="13"/>
+      <c r="AU53" s="13"/>
+      <c r="AV53" s="13"/>
+      <c r="AW53" s="13"/>
+      <c r="AX53" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="AY53" s="17"/>
-      <c r="AZ53" s="17"/>
-      <c r="BA53" s="17"/>
-      <c r="BB53" s="17"/>
-      <c r="BC53" s="17"/>
-      <c r="BD53" s="17"/>
-      <c r="BE53" s="17"/>
-      <c r="BF53" s="18" t="s">
+      <c r="AY53" s="11"/>
+      <c r="AZ53" s="11"/>
+      <c r="BA53" s="11"/>
+      <c r="BB53" s="11"/>
+      <c r="BC53" s="11"/>
+      <c r="BD53" s="11"/>
+      <c r="BE53" s="11"/>
+      <c r="BF53" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="BG53" s="18"/>
-      <c r="BH53" s="18"/>
-      <c r="BI53" s="18"/>
-      <c r="BJ53" s="18"/>
-      <c r="BK53" s="18"/>
-      <c r="BL53" s="18"/>
-      <c r="BM53" s="18"/>
+      <c r="BG53" s="10"/>
+      <c r="BH53" s="10"/>
+      <c r="BI53" s="10"/>
+      <c r="BJ53" s="10"/>
+      <c r="BK53" s="10"/>
+      <c r="BL53" s="10"/>
+      <c r="BM53" s="10"/>
+    </row>
+    <row r="54" spans="2:65" x14ac:dyDescent="0.25">
+      <c r="B54">
+        <v>16</v>
+      </c>
+      <c r="J54">
+        <v>17</v>
+      </c>
+      <c r="R54">
+        <v>18</v>
+      </c>
+      <c r="Z54">
+        <v>19</v>
+      </c>
+      <c r="AH54">
+        <v>20</v>
+      </c>
+      <c r="AP54">
+        <v>21</v>
+      </c>
+      <c r="AX54">
+        <v>22</v>
+      </c>
+      <c r="BF54">
+        <v>23</v>
+      </c>
     </row>
     <row r="55" spans="2:65" x14ac:dyDescent="0.25">
-      <c r="B55" s="11" t="s">
+      <c r="B55" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="C55" s="11"/>
-      <c r="D55" s="11"/>
-      <c r="E55" s="11"/>
-      <c r="F55" s="11"/>
-      <c r="G55" s="11"/>
-      <c r="H55" s="11"/>
-      <c r="I55" s="11"/>
-      <c r="J55" s="12" t="s">
+      <c r="C55" s="17"/>
+      <c r="D55" s="17"/>
+      <c r="E55" s="17"/>
+      <c r="F55" s="17"/>
+      <c r="G55" s="17"/>
+      <c r="H55" s="17"/>
+      <c r="I55" s="17"/>
+      <c r="J55" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="K55" s="12"/>
-      <c r="L55" s="12"/>
-      <c r="M55" s="12"/>
-      <c r="N55" s="12"/>
-      <c r="O55" s="12"/>
-      <c r="P55" s="12"/>
-      <c r="Q55" s="12"/>
-      <c r="R55" s="13" t="s">
+      <c r="K55" s="16"/>
+      <c r="L55" s="16"/>
+      <c r="M55" s="16"/>
+      <c r="N55" s="16"/>
+      <c r="O55" s="16"/>
+      <c r="P55" s="16"/>
+      <c r="Q55" s="16"/>
+      <c r="R55" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="S55" s="13"/>
-      <c r="T55" s="13"/>
-      <c r="U55" s="13"/>
-      <c r="V55" s="13"/>
-      <c r="W55" s="13"/>
-      <c r="X55" s="13"/>
-      <c r="Y55" s="13"/>
-      <c r="Z55" s="14" t="s">
+      <c r="S55" s="14"/>
+      <c r="T55" s="14"/>
+      <c r="U55" s="14"/>
+      <c r="V55" s="14"/>
+      <c r="W55" s="14"/>
+      <c r="X55" s="14"/>
+      <c r="Y55" s="14"/>
+      <c r="Z55" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="AA55" s="14"/>
-      <c r="AB55" s="14"/>
-      <c r="AC55" s="14"/>
-      <c r="AD55" s="14"/>
-      <c r="AE55" s="14"/>
-      <c r="AF55" s="14"/>
-      <c r="AG55" s="14"/>
-      <c r="AH55" s="15" t="s">
+      <c r="AA55" s="15"/>
+      <c r="AB55" s="15"/>
+      <c r="AC55" s="15"/>
+      <c r="AD55" s="15"/>
+      <c r="AE55" s="15"/>
+      <c r="AF55" s="15"/>
+      <c r="AG55" s="15"/>
+      <c r="AH55" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="AI55" s="15"/>
-      <c r="AJ55" s="15"/>
-      <c r="AK55" s="15"/>
-      <c r="AL55" s="15"/>
-      <c r="AM55" s="15"/>
-      <c r="AN55" s="15"/>
-      <c r="AO55" s="15"/>
-      <c r="AP55" s="16" t="s">
+      <c r="AI55" s="12"/>
+      <c r="AJ55" s="12"/>
+      <c r="AK55" s="12"/>
+      <c r="AL55" s="12"/>
+      <c r="AM55" s="12"/>
+      <c r="AN55" s="12"/>
+      <c r="AO55" s="12"/>
+      <c r="AP55" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="AQ55" s="16"/>
-      <c r="AR55" s="16"/>
-      <c r="AS55" s="16"/>
-      <c r="AT55" s="16"/>
-      <c r="AU55" s="16"/>
-      <c r="AV55" s="16"/>
-      <c r="AW55" s="16"/>
-      <c r="AX55" s="17" t="s">
+      <c r="AQ55" s="13"/>
+      <c r="AR55" s="13"/>
+      <c r="AS55" s="13"/>
+      <c r="AT55" s="13"/>
+      <c r="AU55" s="13"/>
+      <c r="AV55" s="13"/>
+      <c r="AW55" s="13"/>
+      <c r="AX55" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="AY55" s="17"/>
-      <c r="AZ55" s="17"/>
-      <c r="BA55" s="17"/>
-      <c r="BB55" s="17"/>
-      <c r="BC55" s="17"/>
-      <c r="BD55" s="17"/>
-      <c r="BE55" s="17"/>
-      <c r="BF55" s="18" t="s">
+      <c r="AY55" s="11"/>
+      <c r="AZ55" s="11"/>
+      <c r="BA55" s="11"/>
+      <c r="BB55" s="11"/>
+      <c r="BC55" s="11"/>
+      <c r="BD55" s="11"/>
+      <c r="BE55" s="11"/>
+      <c r="BF55" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="BG55" s="18"/>
-      <c r="BH55" s="18"/>
-      <c r="BI55" s="18"/>
-      <c r="BJ55" s="18"/>
-      <c r="BK55" s="18"/>
-      <c r="BL55" s="18"/>
-      <c r="BM55" s="18"/>
+      <c r="BG55" s="10"/>
+      <c r="BH55" s="10"/>
+      <c r="BI55" s="10"/>
+      <c r="BJ55" s="10"/>
+      <c r="BK55" s="10"/>
+      <c r="BL55" s="10"/>
+      <c r="BM55" s="10"/>
     </row>
     <row r="57" spans="2:65" x14ac:dyDescent="0.25">
-      <c r="B57" s="11"/>
-      <c r="C57" s="11"/>
-      <c r="D57" s="11"/>
-      <c r="E57" s="11"/>
-      <c r="F57" s="11"/>
-      <c r="G57" s="11"/>
-      <c r="H57" s="11"/>
-      <c r="I57" s="11"/>
-      <c r="J57" s="12"/>
-      <c r="K57" s="12"/>
-      <c r="L57" s="12"/>
-      <c r="M57" s="12"/>
-      <c r="N57" s="12"/>
-      <c r="O57" s="12"/>
-      <c r="P57" s="12"/>
-      <c r="Q57" s="12"/>
-      <c r="R57" s="13"/>
-      <c r="S57" s="13"/>
-      <c r="T57" s="13"/>
-      <c r="U57" s="13"/>
-      <c r="V57" s="13"/>
-      <c r="W57" s="13"/>
-      <c r="X57" s="13"/>
-      <c r="Y57" s="13"/>
-      <c r="Z57" s="14"/>
-      <c r="AA57" s="14"/>
-      <c r="AB57" s="14"/>
-      <c r="AC57" s="14"/>
-      <c r="AD57" s="14"/>
-      <c r="AE57" s="14"/>
-      <c r="AF57" s="14"/>
-      <c r="AG57" s="14"/>
-      <c r="AH57" s="15"/>
-      <c r="AI57" s="15"/>
-      <c r="AJ57" s="15"/>
-      <c r="AK57" s="15"/>
-      <c r="AL57" s="15"/>
-      <c r="AM57" s="15"/>
-      <c r="AN57" s="15"/>
-      <c r="AO57" s="15"/>
-      <c r="AP57" s="16"/>
-      <c r="AQ57" s="16"/>
-      <c r="AR57" s="16"/>
-      <c r="AS57" s="16"/>
-      <c r="AT57" s="16"/>
-      <c r="AU57" s="16"/>
-      <c r="AV57" s="16"/>
-      <c r="AW57" s="16"/>
-      <c r="AX57" s="17"/>
-      <c r="AY57" s="17"/>
-      <c r="AZ57" s="17"/>
-      <c r="BA57" s="17"/>
-      <c r="BB57" s="17"/>
-      <c r="BC57" s="17"/>
-      <c r="BD57" s="17"/>
-      <c r="BE57" s="17"/>
-      <c r="BF57" s="18"/>
-      <c r="BG57" s="18"/>
-      <c r="BH57" s="18"/>
-      <c r="BI57" s="18"/>
-      <c r="BJ57" s="18"/>
-      <c r="BK57" s="18"/>
-      <c r="BL57" s="18"/>
-      <c r="BM57" s="18"/>
+      <c r="B57" s="17"/>
+      <c r="C57" s="17"/>
+      <c r="D57" s="17"/>
+      <c r="E57" s="17"/>
+      <c r="F57" s="17"/>
+      <c r="G57" s="17"/>
+      <c r="H57" s="17"/>
+      <c r="I57" s="17"/>
+      <c r="J57" s="16"/>
+      <c r="K57" s="16"/>
+      <c r="L57" s="16"/>
+      <c r="M57" s="16"/>
+      <c r="N57" s="16"/>
+      <c r="O57" s="16"/>
+      <c r="P57" s="16"/>
+      <c r="Q57" s="16"/>
+      <c r="R57" s="14"/>
+      <c r="S57" s="14"/>
+      <c r="T57" s="14"/>
+      <c r="U57" s="14"/>
+      <c r="V57" s="14"/>
+      <c r="W57" s="14"/>
+      <c r="X57" s="14"/>
+      <c r="Y57" s="14"/>
+      <c r="Z57" s="15"/>
+      <c r="AA57" s="15"/>
+      <c r="AB57" s="15"/>
+      <c r="AC57" s="15"/>
+      <c r="AD57" s="15"/>
+      <c r="AE57" s="15"/>
+      <c r="AF57" s="15"/>
+      <c r="AG57" s="15"/>
+      <c r="AH57" s="12"/>
+      <c r="AI57" s="12"/>
+      <c r="AJ57" s="12"/>
+      <c r="AK57" s="12"/>
+      <c r="AL57" s="12"/>
+      <c r="AM57" s="12"/>
+      <c r="AN57" s="12"/>
+      <c r="AO57" s="12"/>
+      <c r="AP57" s="13"/>
+      <c r="AQ57" s="13"/>
+      <c r="AR57" s="13"/>
+      <c r="AS57" s="13"/>
+      <c r="AT57" s="13"/>
+      <c r="AU57" s="13"/>
+      <c r="AV57" s="13"/>
+      <c r="AW57" s="13"/>
+      <c r="AX57" s="11"/>
+      <c r="AY57" s="11"/>
+      <c r="AZ57" s="11"/>
+      <c r="BA57" s="11"/>
+      <c r="BB57" s="11"/>
+      <c r="BC57" s="11"/>
+      <c r="BD57" s="11"/>
+      <c r="BE57" s="11"/>
+      <c r="BF57" s="10"/>
+      <c r="BG57" s="10"/>
+      <c r="BH57" s="10"/>
+      <c r="BI57" s="10"/>
+      <c r="BJ57" s="10"/>
+      <c r="BK57" s="10"/>
+      <c r="BL57" s="10"/>
+      <c r="BM57" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="71">
-    <mergeCell ref="BF47:BM47"/>
-    <mergeCell ref="BF51:BM51"/>
-    <mergeCell ref="BF53:BM53"/>
-    <mergeCell ref="BF55:BM55"/>
-    <mergeCell ref="BF57:BM57"/>
-    <mergeCell ref="AX45:BE45"/>
-    <mergeCell ref="AX43:BE43"/>
-    <mergeCell ref="AX41:BE41"/>
-    <mergeCell ref="BF41:BM41"/>
-    <mergeCell ref="BF43:BM43"/>
-    <mergeCell ref="BF45:BM45"/>
-    <mergeCell ref="AX57:BE57"/>
-    <mergeCell ref="AX55:BE55"/>
-    <mergeCell ref="AX53:BE53"/>
-    <mergeCell ref="AX51:BE51"/>
-    <mergeCell ref="AX47:BE47"/>
+    <mergeCell ref="X6:AE6"/>
+    <mergeCell ref="BT6:CA6"/>
+    <mergeCell ref="BL6:BS6"/>
+    <mergeCell ref="BD6:BK6"/>
+    <mergeCell ref="AV6:BC6"/>
+    <mergeCell ref="AN6:AU6"/>
+    <mergeCell ref="AF6:AM6"/>
+    <mergeCell ref="B41:I41"/>
+    <mergeCell ref="J43:Q43"/>
+    <mergeCell ref="J41:Q41"/>
+    <mergeCell ref="J45:Q45"/>
+    <mergeCell ref="J47:Q47"/>
+    <mergeCell ref="J51:Q51"/>
+    <mergeCell ref="J53:Q53"/>
+    <mergeCell ref="J55:Q55"/>
+    <mergeCell ref="J57:Q57"/>
+    <mergeCell ref="B43:I43"/>
+    <mergeCell ref="B45:I45"/>
+    <mergeCell ref="B47:I47"/>
+    <mergeCell ref="B51:I51"/>
+    <mergeCell ref="B53:I53"/>
+    <mergeCell ref="B55:I55"/>
+    <mergeCell ref="B57:I57"/>
+    <mergeCell ref="R53:Y53"/>
+    <mergeCell ref="R55:Y55"/>
+    <mergeCell ref="R57:Y57"/>
+    <mergeCell ref="Z41:AG41"/>
+    <mergeCell ref="Z43:AG43"/>
+    <mergeCell ref="Z45:AG45"/>
+    <mergeCell ref="Z47:AG47"/>
+    <mergeCell ref="Z51:AG51"/>
+    <mergeCell ref="Z53:AG53"/>
+    <mergeCell ref="Z55:AG55"/>
+    <mergeCell ref="Z57:AG57"/>
+    <mergeCell ref="R41:Y41"/>
+    <mergeCell ref="R43:Y43"/>
+    <mergeCell ref="R45:Y45"/>
+    <mergeCell ref="R47:Y47"/>
+    <mergeCell ref="R51:Y51"/>
     <mergeCell ref="AH53:AO53"/>
     <mergeCell ref="AH55:AO55"/>
     <mergeCell ref="AH57:AO57"/>
@@ -2797,45 +2898,22 @@
     <mergeCell ref="AH45:AO45"/>
     <mergeCell ref="AH47:AO47"/>
     <mergeCell ref="AH51:AO51"/>
-    <mergeCell ref="R53:Y53"/>
-    <mergeCell ref="R55:Y55"/>
-    <mergeCell ref="R57:Y57"/>
-    <mergeCell ref="Z41:AG41"/>
-    <mergeCell ref="Z43:AG43"/>
-    <mergeCell ref="Z45:AG45"/>
-    <mergeCell ref="Z47:AG47"/>
-    <mergeCell ref="Z51:AG51"/>
-    <mergeCell ref="Z53:AG53"/>
-    <mergeCell ref="Z55:AG55"/>
-    <mergeCell ref="Z57:AG57"/>
-    <mergeCell ref="R41:Y41"/>
-    <mergeCell ref="R43:Y43"/>
-    <mergeCell ref="R45:Y45"/>
-    <mergeCell ref="R47:Y47"/>
-    <mergeCell ref="R51:Y51"/>
-    <mergeCell ref="J51:Q51"/>
-    <mergeCell ref="J53:Q53"/>
-    <mergeCell ref="J55:Q55"/>
-    <mergeCell ref="J57:Q57"/>
-    <mergeCell ref="B43:I43"/>
-    <mergeCell ref="B45:I45"/>
-    <mergeCell ref="B47:I47"/>
-    <mergeCell ref="B51:I51"/>
-    <mergeCell ref="B53:I53"/>
-    <mergeCell ref="B55:I55"/>
-    <mergeCell ref="B57:I57"/>
-    <mergeCell ref="B41:I41"/>
-    <mergeCell ref="J43:Q43"/>
-    <mergeCell ref="J41:Q41"/>
-    <mergeCell ref="J45:Q45"/>
-    <mergeCell ref="J47:Q47"/>
-    <mergeCell ref="X6:AE6"/>
-    <mergeCell ref="BT6:CA6"/>
-    <mergeCell ref="BL6:BS6"/>
-    <mergeCell ref="BD6:BK6"/>
-    <mergeCell ref="AV6:BC6"/>
-    <mergeCell ref="AN6:AU6"/>
-    <mergeCell ref="AF6:AM6"/>
+    <mergeCell ref="AX57:BE57"/>
+    <mergeCell ref="AX55:BE55"/>
+    <mergeCell ref="AX53:BE53"/>
+    <mergeCell ref="AX51:BE51"/>
+    <mergeCell ref="AX47:BE47"/>
+    <mergeCell ref="AX45:BE45"/>
+    <mergeCell ref="AX43:BE43"/>
+    <mergeCell ref="AX41:BE41"/>
+    <mergeCell ref="BF41:BM41"/>
+    <mergeCell ref="BF43:BM43"/>
+    <mergeCell ref="BF45:BM45"/>
+    <mergeCell ref="BF47:BM47"/>
+    <mergeCell ref="BF51:BM51"/>
+    <mergeCell ref="BF53:BM53"/>
+    <mergeCell ref="BF55:BM55"/>
+    <mergeCell ref="BF57:BM57"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Finished everything for APE schwabe primate mutation
</commit_message>
<xml_diff>
--- a/Primates/Mappe1 (Gemt automatisk).xlsx
+++ b/Primates/Mappe1 (Gemt automatisk).xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16729"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -15,7 +15,7 @@
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
     <sheet name="Ark2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="100">
   <si>
     <t>Primate 120:</t>
   </si>
@@ -307,6 +307,24 @@
   </si>
   <si>
     <t>7 left</t>
+  </si>
+  <si>
+    <t>Min egen:</t>
+  </si>
+  <si>
+    <t>En byte indeholdte hel row</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schwabe: </t>
+  </si>
+  <si>
+    <t>En byte indeholder 8 elementer fra en row fra 8 states</t>
+  </si>
+  <si>
+    <t>Rotate en byte</t>
+  </si>
+  <si>
+    <t>shuffle bytes (ingen need for at shuffle på tværs af lanes!!)</t>
   </si>
 </sst>
 </file>
@@ -416,10 +434,17 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -428,19 +453,12 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -534,23 +552,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -586,23 +587,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Kontor">
@@ -755,10 +739,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CA57"/>
+  <dimension ref="A1:CA73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="BB54" sqref="BB54"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J43" sqref="J43:Q43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1650,76 +1634,76 @@
       </c>
     </row>
     <row r="6" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="X6" s="18" t="s">
+      <c r="X6" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="Y6" s="18"/>
-      <c r="Z6" s="18"/>
-      <c r="AA6" s="18"/>
-      <c r="AB6" s="18"/>
-      <c r="AC6" s="18"/>
-      <c r="AD6" s="18"/>
-      <c r="AE6" s="18"/>
-      <c r="AF6" s="18" t="s">
+      <c r="Y6" s="10"/>
+      <c r="Z6" s="10"/>
+      <c r="AA6" s="10"/>
+      <c r="AB6" s="10"/>
+      <c r="AC6" s="10"/>
+      <c r="AD6" s="10"/>
+      <c r="AE6" s="10"/>
+      <c r="AF6" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="AG6" s="18"/>
-      <c r="AH6" s="18"/>
-      <c r="AI6" s="18"/>
-      <c r="AJ6" s="18"/>
-      <c r="AK6" s="18"/>
-      <c r="AL6" s="18"/>
-      <c r="AM6" s="18"/>
-      <c r="AN6" s="18" t="s">
+      <c r="AG6" s="10"/>
+      <c r="AH6" s="10"/>
+      <c r="AI6" s="10"/>
+      <c r="AJ6" s="10"/>
+      <c r="AK6" s="10"/>
+      <c r="AL6" s="10"/>
+      <c r="AM6" s="10"/>
+      <c r="AN6" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="AO6" s="18"/>
-      <c r="AP6" s="18"/>
-      <c r="AQ6" s="18"/>
-      <c r="AR6" s="18"/>
-      <c r="AS6" s="18"/>
-      <c r="AT6" s="18"/>
-      <c r="AU6" s="18"/>
-      <c r="AV6" s="18" t="s">
+      <c r="AO6" s="10"/>
+      <c r="AP6" s="10"/>
+      <c r="AQ6" s="10"/>
+      <c r="AR6" s="10"/>
+      <c r="AS6" s="10"/>
+      <c r="AT6" s="10"/>
+      <c r="AU6" s="10"/>
+      <c r="AV6" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="AW6" s="18"/>
-      <c r="AX6" s="18"/>
-      <c r="AY6" s="18"/>
-      <c r="AZ6" s="18"/>
-      <c r="BA6" s="18"/>
-      <c r="BB6" s="18"/>
-      <c r="BC6" s="18"/>
-      <c r="BD6" s="18" t="s">
+      <c r="AW6" s="10"/>
+      <c r="AX6" s="10"/>
+      <c r="AY6" s="10"/>
+      <c r="AZ6" s="10"/>
+      <c r="BA6" s="10"/>
+      <c r="BB6" s="10"/>
+      <c r="BC6" s="10"/>
+      <c r="BD6" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="BE6" s="18"/>
-      <c r="BF6" s="18"/>
-      <c r="BG6" s="18"/>
-      <c r="BH6" s="18"/>
-      <c r="BI6" s="18"/>
-      <c r="BJ6" s="18"/>
-      <c r="BK6" s="18"/>
-      <c r="BL6" s="18" t="s">
+      <c r="BE6" s="10"/>
+      <c r="BF6" s="10"/>
+      <c r="BG6" s="10"/>
+      <c r="BH6" s="10"/>
+      <c r="BI6" s="10"/>
+      <c r="BJ6" s="10"/>
+      <c r="BK6" s="10"/>
+      <c r="BL6" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="BM6" s="18"/>
-      <c r="BN6" s="18"/>
-      <c r="BO6" s="18"/>
-      <c r="BP6" s="18"/>
-      <c r="BQ6" s="18"/>
-      <c r="BR6" s="18"/>
-      <c r="BS6" s="18"/>
-      <c r="BT6" s="18" t="s">
+      <c r="BM6" s="10"/>
+      <c r="BN6" s="10"/>
+      <c r="BO6" s="10"/>
+      <c r="BP6" s="10"/>
+      <c r="BQ6" s="10"/>
+      <c r="BR6" s="10"/>
+      <c r="BS6" s="10"/>
+      <c r="BT6" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="BU6" s="18"/>
-      <c r="BV6" s="18"/>
-      <c r="BW6" s="18"/>
-      <c r="BX6" s="18"/>
-      <c r="BY6" s="18"/>
-      <c r="BZ6" s="18"/>
-      <c r="CA6" s="18"/>
+      <c r="BU6" s="10"/>
+      <c r="BV6" s="10"/>
+      <c r="BW6" s="10"/>
+      <c r="BX6" s="10"/>
+      <c r="BY6" s="10"/>
+      <c r="BZ6" s="10"/>
+      <c r="CA6" s="10"/>
     </row>
     <row r="8" spans="1:79" x14ac:dyDescent="0.25">
       <c r="AF8" t="s">
@@ -2124,332 +2108,332 @@
       </c>
     </row>
     <row r="41" spans="1:65" x14ac:dyDescent="0.25">
-      <c r="B41" s="17" t="s">
+      <c r="B41" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C41" s="17"/>
-      <c r="D41" s="17"/>
-      <c r="E41" s="17"/>
-      <c r="F41" s="17"/>
-      <c r="G41" s="17"/>
-      <c r="H41" s="17"/>
-      <c r="I41" s="17"/>
-      <c r="J41" s="16" t="s">
+      <c r="C41" s="11"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="11"/>
+      <c r="H41" s="11"/>
+      <c r="I41" s="11"/>
+      <c r="J41" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="K41" s="16"/>
-      <c r="L41" s="16"/>
-      <c r="M41" s="16"/>
-      <c r="N41" s="16"/>
-      <c r="O41" s="16"/>
-      <c r="P41" s="16"/>
-      <c r="Q41" s="16"/>
-      <c r="R41" s="14" t="s">
+      <c r="K41" s="12"/>
+      <c r="L41" s="12"/>
+      <c r="M41" s="12"/>
+      <c r="N41" s="12"/>
+      <c r="O41" s="12"/>
+      <c r="P41" s="12"/>
+      <c r="Q41" s="12"/>
+      <c r="R41" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="S41" s="14"/>
-      <c r="T41" s="14"/>
-      <c r="U41" s="14"/>
-      <c r="V41" s="14"/>
-      <c r="W41" s="14"/>
-      <c r="X41" s="14"/>
-      <c r="Y41" s="14"/>
-      <c r="Z41" s="15" t="s">
+      <c r="S41" s="13"/>
+      <c r="T41" s="13"/>
+      <c r="U41" s="13"/>
+      <c r="V41" s="13"/>
+      <c r="W41" s="13"/>
+      <c r="X41" s="13"/>
+      <c r="Y41" s="13"/>
+      <c r="Z41" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="AA41" s="15"/>
-      <c r="AB41" s="15"/>
-      <c r="AC41" s="15"/>
-      <c r="AD41" s="15"/>
-      <c r="AE41" s="15"/>
-      <c r="AF41" s="15"/>
-      <c r="AG41" s="15"/>
-      <c r="AH41" s="12" t="s">
+      <c r="AA41" s="14"/>
+      <c r="AB41" s="14"/>
+      <c r="AC41" s="14"/>
+      <c r="AD41" s="14"/>
+      <c r="AE41" s="14"/>
+      <c r="AF41" s="14"/>
+      <c r="AG41" s="14"/>
+      <c r="AH41" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="AI41" s="12"/>
-      <c r="AJ41" s="12"/>
-      <c r="AK41" s="12"/>
-      <c r="AL41" s="12"/>
-      <c r="AM41" s="12"/>
-      <c r="AN41" s="12"/>
-      <c r="AO41" s="12"/>
-      <c r="AP41" s="13" t="s">
+      <c r="AI41" s="15"/>
+      <c r="AJ41" s="15"/>
+      <c r="AK41" s="15"/>
+      <c r="AL41" s="15"/>
+      <c r="AM41" s="15"/>
+      <c r="AN41" s="15"/>
+      <c r="AO41" s="15"/>
+      <c r="AP41" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="AQ41" s="13"/>
-      <c r="AR41" s="13"/>
-      <c r="AS41" s="13"/>
-      <c r="AT41" s="13"/>
-      <c r="AU41" s="13"/>
-      <c r="AV41" s="13"/>
-      <c r="AW41" s="13"/>
-      <c r="AX41" s="11" t="s">
+      <c r="AQ41" s="16"/>
+      <c r="AR41" s="16"/>
+      <c r="AS41" s="16"/>
+      <c r="AT41" s="16"/>
+      <c r="AU41" s="16"/>
+      <c r="AV41" s="16"/>
+      <c r="AW41" s="16"/>
+      <c r="AX41" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="AY41" s="11"/>
-      <c r="AZ41" s="11"/>
-      <c r="BA41" s="11"/>
-      <c r="BB41" s="11"/>
-      <c r="BC41" s="11"/>
-      <c r="BD41" s="11"/>
-      <c r="BE41" s="11"/>
-      <c r="BF41" s="10" t="s">
+      <c r="AY41" s="17"/>
+      <c r="AZ41" s="17"/>
+      <c r="BA41" s="17"/>
+      <c r="BB41" s="17"/>
+      <c r="BC41" s="17"/>
+      <c r="BD41" s="17"/>
+      <c r="BE41" s="17"/>
+      <c r="BF41" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="BG41" s="10"/>
-      <c r="BH41" s="10"/>
-      <c r="BI41" s="10"/>
-      <c r="BJ41" s="10"/>
-      <c r="BK41" s="10"/>
-      <c r="BL41" s="10"/>
-      <c r="BM41" s="10"/>
+      <c r="BG41" s="18"/>
+      <c r="BH41" s="18"/>
+      <c r="BI41" s="18"/>
+      <c r="BJ41" s="18"/>
+      <c r="BK41" s="18"/>
+      <c r="BL41" s="18"/>
+      <c r="BM41" s="18"/>
     </row>
     <row r="43" spans="1:65" x14ac:dyDescent="0.25">
-      <c r="B43" s="17" t="s">
+      <c r="B43" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C43" s="17"/>
-      <c r="D43" s="17"/>
-      <c r="E43" s="17"/>
-      <c r="F43" s="17"/>
-      <c r="G43" s="17"/>
-      <c r="H43" s="17"/>
-      <c r="I43" s="17"/>
-      <c r="J43" s="16" t="s">
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
+      <c r="E43" s="11"/>
+      <c r="F43" s="11"/>
+      <c r="G43" s="11"/>
+      <c r="H43" s="11"/>
+      <c r="I43" s="11"/>
+      <c r="J43" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="K43" s="16"/>
-      <c r="L43" s="16"/>
-      <c r="M43" s="16"/>
-      <c r="N43" s="16"/>
-      <c r="O43" s="16"/>
-      <c r="P43" s="16"/>
-      <c r="Q43" s="16"/>
-      <c r="R43" s="14" t="s">
+      <c r="K43" s="12"/>
+      <c r="L43" s="12"/>
+      <c r="M43" s="12"/>
+      <c r="N43" s="12"/>
+      <c r="O43" s="12"/>
+      <c r="P43" s="12"/>
+      <c r="Q43" s="12"/>
+      <c r="R43" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="S43" s="14"/>
-      <c r="T43" s="14"/>
-      <c r="U43" s="14"/>
-      <c r="V43" s="14"/>
-      <c r="W43" s="14"/>
-      <c r="X43" s="14"/>
-      <c r="Y43" s="14"/>
-      <c r="Z43" s="15" t="s">
+      <c r="S43" s="13"/>
+      <c r="T43" s="13"/>
+      <c r="U43" s="13"/>
+      <c r="V43" s="13"/>
+      <c r="W43" s="13"/>
+      <c r="X43" s="13"/>
+      <c r="Y43" s="13"/>
+      <c r="Z43" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="AA43" s="15"/>
-      <c r="AB43" s="15"/>
-      <c r="AC43" s="15"/>
-      <c r="AD43" s="15"/>
-      <c r="AE43" s="15"/>
-      <c r="AF43" s="15"/>
-      <c r="AG43" s="15"/>
-      <c r="AH43" s="12" t="s">
+      <c r="AA43" s="14"/>
+      <c r="AB43" s="14"/>
+      <c r="AC43" s="14"/>
+      <c r="AD43" s="14"/>
+      <c r="AE43" s="14"/>
+      <c r="AF43" s="14"/>
+      <c r="AG43" s="14"/>
+      <c r="AH43" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="AI43" s="12"/>
-      <c r="AJ43" s="12"/>
-      <c r="AK43" s="12"/>
-      <c r="AL43" s="12"/>
-      <c r="AM43" s="12"/>
-      <c r="AN43" s="12"/>
-      <c r="AO43" s="12"/>
-      <c r="AP43" s="13" t="s">
+      <c r="AI43" s="15"/>
+      <c r="AJ43" s="15"/>
+      <c r="AK43" s="15"/>
+      <c r="AL43" s="15"/>
+      <c r="AM43" s="15"/>
+      <c r="AN43" s="15"/>
+      <c r="AO43" s="15"/>
+      <c r="AP43" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="AQ43" s="13"/>
-      <c r="AR43" s="13"/>
-      <c r="AS43" s="13"/>
-      <c r="AT43" s="13"/>
-      <c r="AU43" s="13"/>
-      <c r="AV43" s="13"/>
-      <c r="AW43" s="13"/>
-      <c r="AX43" s="11" t="s">
+      <c r="AQ43" s="16"/>
+      <c r="AR43" s="16"/>
+      <c r="AS43" s="16"/>
+      <c r="AT43" s="16"/>
+      <c r="AU43" s="16"/>
+      <c r="AV43" s="16"/>
+      <c r="AW43" s="16"/>
+      <c r="AX43" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="AY43" s="11"/>
-      <c r="AZ43" s="11"/>
-      <c r="BA43" s="11"/>
-      <c r="BB43" s="11"/>
-      <c r="BC43" s="11"/>
-      <c r="BD43" s="11"/>
-      <c r="BE43" s="11"/>
-      <c r="BF43" s="10" t="s">
+      <c r="AY43" s="17"/>
+      <c r="AZ43" s="17"/>
+      <c r="BA43" s="17"/>
+      <c r="BB43" s="17"/>
+      <c r="BC43" s="17"/>
+      <c r="BD43" s="17"/>
+      <c r="BE43" s="17"/>
+      <c r="BF43" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="BG43" s="10"/>
-      <c r="BH43" s="10"/>
-      <c r="BI43" s="10"/>
-      <c r="BJ43" s="10"/>
-      <c r="BK43" s="10"/>
-      <c r="BL43" s="10"/>
-      <c r="BM43" s="10"/>
+      <c r="BG43" s="18"/>
+      <c r="BH43" s="18"/>
+      <c r="BI43" s="18"/>
+      <c r="BJ43" s="18"/>
+      <c r="BK43" s="18"/>
+      <c r="BL43" s="18"/>
+      <c r="BM43" s="18"/>
     </row>
     <row r="45" spans="1:65" x14ac:dyDescent="0.25">
-      <c r="B45" s="17" t="s">
+      <c r="B45" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C45" s="17"/>
-      <c r="D45" s="17"/>
-      <c r="E45" s="17"/>
-      <c r="F45" s="17"/>
-      <c r="G45" s="17"/>
-      <c r="H45" s="17"/>
-      <c r="I45" s="17"/>
-      <c r="J45" s="16" t="s">
+      <c r="C45" s="11"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="11"/>
+      <c r="G45" s="11"/>
+      <c r="H45" s="11"/>
+      <c r="I45" s="11"/>
+      <c r="J45" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="K45" s="16"/>
-      <c r="L45" s="16"/>
-      <c r="M45" s="16"/>
-      <c r="N45" s="16"/>
-      <c r="O45" s="16"/>
-      <c r="P45" s="16"/>
-      <c r="Q45" s="16"/>
-      <c r="R45" s="14" t="s">
+      <c r="K45" s="12"/>
+      <c r="L45" s="12"/>
+      <c r="M45" s="12"/>
+      <c r="N45" s="12"/>
+      <c r="O45" s="12"/>
+      <c r="P45" s="12"/>
+      <c r="Q45" s="12"/>
+      <c r="R45" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="S45" s="14"/>
-      <c r="T45" s="14"/>
-      <c r="U45" s="14"/>
-      <c r="V45" s="14"/>
-      <c r="W45" s="14"/>
-      <c r="X45" s="14"/>
-      <c r="Y45" s="14"/>
-      <c r="Z45" s="15" t="s">
+      <c r="S45" s="13"/>
+      <c r="T45" s="13"/>
+      <c r="U45" s="13"/>
+      <c r="V45" s="13"/>
+      <c r="W45" s="13"/>
+      <c r="X45" s="13"/>
+      <c r="Y45" s="13"/>
+      <c r="Z45" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="AA45" s="15"/>
-      <c r="AB45" s="15"/>
-      <c r="AC45" s="15"/>
-      <c r="AD45" s="15"/>
-      <c r="AE45" s="15"/>
-      <c r="AF45" s="15"/>
-      <c r="AG45" s="15"/>
-      <c r="AH45" s="12" t="s">
+      <c r="AA45" s="14"/>
+      <c r="AB45" s="14"/>
+      <c r="AC45" s="14"/>
+      <c r="AD45" s="14"/>
+      <c r="AE45" s="14"/>
+      <c r="AF45" s="14"/>
+      <c r="AG45" s="14"/>
+      <c r="AH45" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="AI45" s="12"/>
-      <c r="AJ45" s="12"/>
-      <c r="AK45" s="12"/>
-      <c r="AL45" s="12"/>
-      <c r="AM45" s="12"/>
-      <c r="AN45" s="12"/>
-      <c r="AO45" s="12"/>
-      <c r="AP45" s="13" t="s">
+      <c r="AI45" s="15"/>
+      <c r="AJ45" s="15"/>
+      <c r="AK45" s="15"/>
+      <c r="AL45" s="15"/>
+      <c r="AM45" s="15"/>
+      <c r="AN45" s="15"/>
+      <c r="AO45" s="15"/>
+      <c r="AP45" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="AQ45" s="13"/>
-      <c r="AR45" s="13"/>
-      <c r="AS45" s="13"/>
-      <c r="AT45" s="13"/>
-      <c r="AU45" s="13"/>
-      <c r="AV45" s="13"/>
-      <c r="AW45" s="13"/>
-      <c r="AX45" s="11" t="s">
+      <c r="AQ45" s="16"/>
+      <c r="AR45" s="16"/>
+      <c r="AS45" s="16"/>
+      <c r="AT45" s="16"/>
+      <c r="AU45" s="16"/>
+      <c r="AV45" s="16"/>
+      <c r="AW45" s="16"/>
+      <c r="AX45" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="AY45" s="11"/>
-      <c r="AZ45" s="11"/>
-      <c r="BA45" s="11"/>
-      <c r="BB45" s="11"/>
-      <c r="BC45" s="11"/>
-      <c r="BD45" s="11"/>
-      <c r="BE45" s="11"/>
-      <c r="BF45" s="10" t="s">
+      <c r="AY45" s="17"/>
+      <c r="AZ45" s="17"/>
+      <c r="BA45" s="17"/>
+      <c r="BB45" s="17"/>
+      <c r="BC45" s="17"/>
+      <c r="BD45" s="17"/>
+      <c r="BE45" s="17"/>
+      <c r="BF45" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="BG45" s="10"/>
-      <c r="BH45" s="10"/>
-      <c r="BI45" s="10"/>
-      <c r="BJ45" s="10"/>
-      <c r="BK45" s="10"/>
-      <c r="BL45" s="10"/>
-      <c r="BM45" s="10"/>
+      <c r="BG45" s="18"/>
+      <c r="BH45" s="18"/>
+      <c r="BI45" s="18"/>
+      <c r="BJ45" s="18"/>
+      <c r="BK45" s="18"/>
+      <c r="BL45" s="18"/>
+      <c r="BM45" s="18"/>
     </row>
     <row r="47" spans="1:65" x14ac:dyDescent="0.25">
-      <c r="B47" s="17" t="s">
+      <c r="B47" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="C47" s="17"/>
-      <c r="D47" s="17"/>
-      <c r="E47" s="17"/>
-      <c r="F47" s="17"/>
-      <c r="G47" s="17"/>
-      <c r="H47" s="17"/>
-      <c r="I47" s="17"/>
-      <c r="J47" s="16" t="s">
+      <c r="C47" s="11"/>
+      <c r="D47" s="11"/>
+      <c r="E47" s="11"/>
+      <c r="F47" s="11"/>
+      <c r="G47" s="11"/>
+      <c r="H47" s="11"/>
+      <c r="I47" s="11"/>
+      <c r="J47" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="K47" s="16"/>
-      <c r="L47" s="16"/>
-      <c r="M47" s="16"/>
-      <c r="N47" s="16"/>
-      <c r="O47" s="16"/>
-      <c r="P47" s="16"/>
-      <c r="Q47" s="16"/>
-      <c r="R47" s="14" t="s">
+      <c r="K47" s="12"/>
+      <c r="L47" s="12"/>
+      <c r="M47" s="12"/>
+      <c r="N47" s="12"/>
+      <c r="O47" s="12"/>
+      <c r="P47" s="12"/>
+      <c r="Q47" s="12"/>
+      <c r="R47" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="S47" s="14"/>
-      <c r="T47" s="14"/>
-      <c r="U47" s="14"/>
-      <c r="V47" s="14"/>
-      <c r="W47" s="14"/>
-      <c r="X47" s="14"/>
-      <c r="Y47" s="14"/>
-      <c r="Z47" s="15" t="s">
+      <c r="S47" s="13"/>
+      <c r="T47" s="13"/>
+      <c r="U47" s="13"/>
+      <c r="V47" s="13"/>
+      <c r="W47" s="13"/>
+      <c r="X47" s="13"/>
+      <c r="Y47" s="13"/>
+      <c r="Z47" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="AA47" s="15"/>
-      <c r="AB47" s="15"/>
-      <c r="AC47" s="15"/>
-      <c r="AD47" s="15"/>
-      <c r="AE47" s="15"/>
-      <c r="AF47" s="15"/>
-      <c r="AG47" s="15"/>
-      <c r="AH47" s="12" t="s">
+      <c r="AA47" s="14"/>
+      <c r="AB47" s="14"/>
+      <c r="AC47" s="14"/>
+      <c r="AD47" s="14"/>
+      <c r="AE47" s="14"/>
+      <c r="AF47" s="14"/>
+      <c r="AG47" s="14"/>
+      <c r="AH47" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="AI47" s="12"/>
-      <c r="AJ47" s="12"/>
-      <c r="AK47" s="12"/>
-      <c r="AL47" s="12"/>
-      <c r="AM47" s="12"/>
-      <c r="AN47" s="12"/>
-      <c r="AO47" s="12"/>
-      <c r="AP47" s="13" t="s">
+      <c r="AI47" s="15"/>
+      <c r="AJ47" s="15"/>
+      <c r="AK47" s="15"/>
+      <c r="AL47" s="15"/>
+      <c r="AM47" s="15"/>
+      <c r="AN47" s="15"/>
+      <c r="AO47" s="15"/>
+      <c r="AP47" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="AQ47" s="13"/>
-      <c r="AR47" s="13"/>
-      <c r="AS47" s="13"/>
-      <c r="AT47" s="13"/>
-      <c r="AU47" s="13"/>
-      <c r="AV47" s="13"/>
-      <c r="AW47" s="13"/>
-      <c r="AX47" s="11" t="s">
+      <c r="AQ47" s="16"/>
+      <c r="AR47" s="16"/>
+      <c r="AS47" s="16"/>
+      <c r="AT47" s="16"/>
+      <c r="AU47" s="16"/>
+      <c r="AV47" s="16"/>
+      <c r="AW47" s="16"/>
+      <c r="AX47" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="AY47" s="11"/>
-      <c r="AZ47" s="11"/>
-      <c r="BA47" s="11"/>
-      <c r="BB47" s="11"/>
-      <c r="BC47" s="11"/>
-      <c r="BD47" s="11"/>
-      <c r="BE47" s="11"/>
-      <c r="BF47" s="10" t="s">
+      <c r="AY47" s="17"/>
+      <c r="AZ47" s="17"/>
+      <c r="BA47" s="17"/>
+      <c r="BB47" s="17"/>
+      <c r="BC47" s="17"/>
+      <c r="BD47" s="17"/>
+      <c r="BE47" s="17"/>
+      <c r="BF47" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="BG47" s="10"/>
-      <c r="BH47" s="10"/>
-      <c r="BI47" s="10"/>
-      <c r="BJ47" s="10"/>
-      <c r="BK47" s="10"/>
-      <c r="BL47" s="10"/>
-      <c r="BM47" s="10"/>
+      <c r="BG47" s="18"/>
+      <c r="BH47" s="18"/>
+      <c r="BI47" s="18"/>
+      <c r="BJ47" s="18"/>
+      <c r="BK47" s="18"/>
+      <c r="BL47" s="18"/>
+      <c r="BM47" s="18"/>
     </row>
     <row r="50" spans="2:65" x14ac:dyDescent="0.25">
       <c r="B50">
@@ -2478,86 +2462,86 @@
       </c>
     </row>
     <row r="51" spans="2:65" x14ac:dyDescent="0.25">
-      <c r="B51" s="17" t="s">
+      <c r="B51" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="C51" s="17"/>
-      <c r="D51" s="17"/>
-      <c r="E51" s="17"/>
-      <c r="F51" s="17"/>
-      <c r="G51" s="17"/>
-      <c r="H51" s="17"/>
-      <c r="I51" s="17"/>
-      <c r="J51" s="16" t="s">
+      <c r="C51" s="11"/>
+      <c r="D51" s="11"/>
+      <c r="E51" s="11"/>
+      <c r="F51" s="11"/>
+      <c r="G51" s="11"/>
+      <c r="H51" s="11"/>
+      <c r="I51" s="11"/>
+      <c r="J51" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="K51" s="16"/>
-      <c r="L51" s="16"/>
-      <c r="M51" s="16"/>
-      <c r="N51" s="16"/>
-      <c r="O51" s="16"/>
-      <c r="P51" s="16"/>
-      <c r="Q51" s="16"/>
-      <c r="R51" s="14" t="s">
+      <c r="K51" s="12"/>
+      <c r="L51" s="12"/>
+      <c r="M51" s="12"/>
+      <c r="N51" s="12"/>
+      <c r="O51" s="12"/>
+      <c r="P51" s="12"/>
+      <c r="Q51" s="12"/>
+      <c r="R51" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="S51" s="14"/>
-      <c r="T51" s="14"/>
-      <c r="U51" s="14"/>
-      <c r="V51" s="14"/>
-      <c r="W51" s="14"/>
-      <c r="X51" s="14"/>
-      <c r="Y51" s="14"/>
-      <c r="Z51" s="15" t="s">
+      <c r="S51" s="13"/>
+      <c r="T51" s="13"/>
+      <c r="U51" s="13"/>
+      <c r="V51" s="13"/>
+      <c r="W51" s="13"/>
+      <c r="X51" s="13"/>
+      <c r="Y51" s="13"/>
+      <c r="Z51" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="AA51" s="15"/>
-      <c r="AB51" s="15"/>
-      <c r="AC51" s="15"/>
-      <c r="AD51" s="15"/>
-      <c r="AE51" s="15"/>
-      <c r="AF51" s="15"/>
-      <c r="AG51" s="15"/>
-      <c r="AH51" s="12" t="s">
+      <c r="AA51" s="14"/>
+      <c r="AB51" s="14"/>
+      <c r="AC51" s="14"/>
+      <c r="AD51" s="14"/>
+      <c r="AE51" s="14"/>
+      <c r="AF51" s="14"/>
+      <c r="AG51" s="14"/>
+      <c r="AH51" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="AI51" s="12"/>
-      <c r="AJ51" s="12"/>
-      <c r="AK51" s="12"/>
-      <c r="AL51" s="12"/>
-      <c r="AM51" s="12"/>
-      <c r="AN51" s="12"/>
-      <c r="AO51" s="12"/>
-      <c r="AP51" s="13" t="s">
+      <c r="AI51" s="15"/>
+      <c r="AJ51" s="15"/>
+      <c r="AK51" s="15"/>
+      <c r="AL51" s="15"/>
+      <c r="AM51" s="15"/>
+      <c r="AN51" s="15"/>
+      <c r="AO51" s="15"/>
+      <c r="AP51" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="AQ51" s="13"/>
-      <c r="AR51" s="13"/>
-      <c r="AS51" s="13"/>
-      <c r="AT51" s="13"/>
-      <c r="AU51" s="13"/>
-      <c r="AV51" s="13"/>
-      <c r="AW51" s="13"/>
-      <c r="AX51" s="11" t="s">
+      <c r="AQ51" s="16"/>
+      <c r="AR51" s="16"/>
+      <c r="AS51" s="16"/>
+      <c r="AT51" s="16"/>
+      <c r="AU51" s="16"/>
+      <c r="AV51" s="16"/>
+      <c r="AW51" s="16"/>
+      <c r="AX51" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="AY51" s="11"/>
-      <c r="AZ51" s="11"/>
-      <c r="BA51" s="11"/>
-      <c r="BB51" s="11"/>
-      <c r="BC51" s="11"/>
-      <c r="BD51" s="11"/>
-      <c r="BE51" s="11"/>
-      <c r="BF51" s="10" t="s">
+      <c r="AY51" s="17"/>
+      <c r="AZ51" s="17"/>
+      <c r="BA51" s="17"/>
+      <c r="BB51" s="17"/>
+      <c r="BC51" s="17"/>
+      <c r="BD51" s="17"/>
+      <c r="BE51" s="17"/>
+      <c r="BF51" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="BG51" s="10"/>
-      <c r="BH51" s="10"/>
-      <c r="BI51" s="10"/>
-      <c r="BJ51" s="10"/>
-      <c r="BK51" s="10"/>
-      <c r="BL51" s="10"/>
-      <c r="BM51" s="10"/>
+      <c r="BG51" s="18"/>
+      <c r="BH51" s="18"/>
+      <c r="BI51" s="18"/>
+      <c r="BJ51" s="18"/>
+      <c r="BK51" s="18"/>
+      <c r="BL51" s="18"/>
+      <c r="BM51" s="18"/>
     </row>
     <row r="52" spans="2:65" x14ac:dyDescent="0.25">
       <c r="B52">
@@ -2586,86 +2570,86 @@
       </c>
     </row>
     <row r="53" spans="2:65" x14ac:dyDescent="0.25">
-      <c r="B53" s="17" t="s">
+      <c r="B53" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="C53" s="17"/>
-      <c r="D53" s="17"/>
-      <c r="E53" s="17"/>
-      <c r="F53" s="17"/>
-      <c r="G53" s="17"/>
-      <c r="H53" s="17"/>
-      <c r="I53" s="17"/>
-      <c r="J53" s="16" t="s">
+      <c r="C53" s="11"/>
+      <c r="D53" s="11"/>
+      <c r="E53" s="11"/>
+      <c r="F53" s="11"/>
+      <c r="G53" s="11"/>
+      <c r="H53" s="11"/>
+      <c r="I53" s="11"/>
+      <c r="J53" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="K53" s="16"/>
-      <c r="L53" s="16"/>
-      <c r="M53" s="16"/>
-      <c r="N53" s="16"/>
-      <c r="O53" s="16"/>
-      <c r="P53" s="16"/>
-      <c r="Q53" s="16"/>
-      <c r="R53" s="14" t="s">
+      <c r="K53" s="12"/>
+      <c r="L53" s="12"/>
+      <c r="M53" s="12"/>
+      <c r="N53" s="12"/>
+      <c r="O53" s="12"/>
+      <c r="P53" s="12"/>
+      <c r="Q53" s="12"/>
+      <c r="R53" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="S53" s="14"/>
-      <c r="T53" s="14"/>
-      <c r="U53" s="14"/>
-      <c r="V53" s="14"/>
-      <c r="W53" s="14"/>
-      <c r="X53" s="14"/>
-      <c r="Y53" s="14"/>
-      <c r="Z53" s="15" t="s">
+      <c r="S53" s="13"/>
+      <c r="T53" s="13"/>
+      <c r="U53" s="13"/>
+      <c r="V53" s="13"/>
+      <c r="W53" s="13"/>
+      <c r="X53" s="13"/>
+      <c r="Y53" s="13"/>
+      <c r="Z53" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="AA53" s="15"/>
-      <c r="AB53" s="15"/>
-      <c r="AC53" s="15"/>
-      <c r="AD53" s="15"/>
-      <c r="AE53" s="15"/>
-      <c r="AF53" s="15"/>
-      <c r="AG53" s="15"/>
-      <c r="AH53" s="12" t="s">
+      <c r="AA53" s="14"/>
+      <c r="AB53" s="14"/>
+      <c r="AC53" s="14"/>
+      <c r="AD53" s="14"/>
+      <c r="AE53" s="14"/>
+      <c r="AF53" s="14"/>
+      <c r="AG53" s="14"/>
+      <c r="AH53" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="AI53" s="12"/>
-      <c r="AJ53" s="12"/>
-      <c r="AK53" s="12"/>
-      <c r="AL53" s="12"/>
-      <c r="AM53" s="12"/>
-      <c r="AN53" s="12"/>
-      <c r="AO53" s="12"/>
-      <c r="AP53" s="13" t="s">
+      <c r="AI53" s="15"/>
+      <c r="AJ53" s="15"/>
+      <c r="AK53" s="15"/>
+      <c r="AL53" s="15"/>
+      <c r="AM53" s="15"/>
+      <c r="AN53" s="15"/>
+      <c r="AO53" s="15"/>
+      <c r="AP53" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="AQ53" s="13"/>
-      <c r="AR53" s="13"/>
-      <c r="AS53" s="13"/>
-      <c r="AT53" s="13"/>
-      <c r="AU53" s="13"/>
-      <c r="AV53" s="13"/>
-      <c r="AW53" s="13"/>
-      <c r="AX53" s="11" t="s">
+      <c r="AQ53" s="16"/>
+      <c r="AR53" s="16"/>
+      <c r="AS53" s="16"/>
+      <c r="AT53" s="16"/>
+      <c r="AU53" s="16"/>
+      <c r="AV53" s="16"/>
+      <c r="AW53" s="16"/>
+      <c r="AX53" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="AY53" s="11"/>
-      <c r="AZ53" s="11"/>
-      <c r="BA53" s="11"/>
-      <c r="BB53" s="11"/>
-      <c r="BC53" s="11"/>
-      <c r="BD53" s="11"/>
-      <c r="BE53" s="11"/>
-      <c r="BF53" s="10" t="s">
+      <c r="AY53" s="17"/>
+      <c r="AZ53" s="17"/>
+      <c r="BA53" s="17"/>
+      <c r="BB53" s="17"/>
+      <c r="BC53" s="17"/>
+      <c r="BD53" s="17"/>
+      <c r="BE53" s="17"/>
+      <c r="BF53" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="BG53" s="10"/>
-      <c r="BH53" s="10"/>
-      <c r="BI53" s="10"/>
-      <c r="BJ53" s="10"/>
-      <c r="BK53" s="10"/>
-      <c r="BL53" s="10"/>
-      <c r="BM53" s="10"/>
+      <c r="BG53" s="18"/>
+      <c r="BH53" s="18"/>
+      <c r="BI53" s="18"/>
+      <c r="BJ53" s="18"/>
+      <c r="BK53" s="18"/>
+      <c r="BL53" s="18"/>
+      <c r="BM53" s="18"/>
     </row>
     <row r="54" spans="2:65" x14ac:dyDescent="0.25">
       <c r="B54">
@@ -2694,178 +2678,248 @@
       </c>
     </row>
     <row r="55" spans="2:65" x14ac:dyDescent="0.25">
-      <c r="B55" s="17" t="s">
+      <c r="B55" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="C55" s="17"/>
-      <c r="D55" s="17"/>
-      <c r="E55" s="17"/>
-      <c r="F55" s="17"/>
-      <c r="G55" s="17"/>
-      <c r="H55" s="17"/>
-      <c r="I55" s="17"/>
-      <c r="J55" s="16" t="s">
+      <c r="C55" s="11"/>
+      <c r="D55" s="11"/>
+      <c r="E55" s="11"/>
+      <c r="F55" s="11"/>
+      <c r="G55" s="11"/>
+      <c r="H55" s="11"/>
+      <c r="I55" s="11"/>
+      <c r="J55" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="K55" s="16"/>
-      <c r="L55" s="16"/>
-      <c r="M55" s="16"/>
-      <c r="N55" s="16"/>
-      <c r="O55" s="16"/>
-      <c r="P55" s="16"/>
-      <c r="Q55" s="16"/>
-      <c r="R55" s="14" t="s">
+      <c r="K55" s="12"/>
+      <c r="L55" s="12"/>
+      <c r="M55" s="12"/>
+      <c r="N55" s="12"/>
+      <c r="O55" s="12"/>
+      <c r="P55" s="12"/>
+      <c r="Q55" s="12"/>
+      <c r="R55" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="S55" s="14"/>
-      <c r="T55" s="14"/>
-      <c r="U55" s="14"/>
-      <c r="V55" s="14"/>
-      <c r="W55" s="14"/>
-      <c r="X55" s="14"/>
-      <c r="Y55" s="14"/>
-      <c r="Z55" s="15" t="s">
+      <c r="S55" s="13"/>
+      <c r="T55" s="13"/>
+      <c r="U55" s="13"/>
+      <c r="V55" s="13"/>
+      <c r="W55" s="13"/>
+      <c r="X55" s="13"/>
+      <c r="Y55" s="13"/>
+      <c r="Z55" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="AA55" s="15"/>
-      <c r="AB55" s="15"/>
-      <c r="AC55" s="15"/>
-      <c r="AD55" s="15"/>
-      <c r="AE55" s="15"/>
-      <c r="AF55" s="15"/>
-      <c r="AG55" s="15"/>
-      <c r="AH55" s="12" t="s">
+      <c r="AA55" s="14"/>
+      <c r="AB55" s="14"/>
+      <c r="AC55" s="14"/>
+      <c r="AD55" s="14"/>
+      <c r="AE55" s="14"/>
+      <c r="AF55" s="14"/>
+      <c r="AG55" s="14"/>
+      <c r="AH55" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="AI55" s="12"/>
-      <c r="AJ55" s="12"/>
-      <c r="AK55" s="12"/>
-      <c r="AL55" s="12"/>
-      <c r="AM55" s="12"/>
-      <c r="AN55" s="12"/>
-      <c r="AO55" s="12"/>
-      <c r="AP55" s="13" t="s">
+      <c r="AI55" s="15"/>
+      <c r="AJ55" s="15"/>
+      <c r="AK55" s="15"/>
+      <c r="AL55" s="15"/>
+      <c r="AM55" s="15"/>
+      <c r="AN55" s="15"/>
+      <c r="AO55" s="15"/>
+      <c r="AP55" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="AQ55" s="13"/>
-      <c r="AR55" s="13"/>
-      <c r="AS55" s="13"/>
-      <c r="AT55" s="13"/>
-      <c r="AU55" s="13"/>
-      <c r="AV55" s="13"/>
-      <c r="AW55" s="13"/>
-      <c r="AX55" s="11" t="s">
+      <c r="AQ55" s="16"/>
+      <c r="AR55" s="16"/>
+      <c r="AS55" s="16"/>
+      <c r="AT55" s="16"/>
+      <c r="AU55" s="16"/>
+      <c r="AV55" s="16"/>
+      <c r="AW55" s="16"/>
+      <c r="AX55" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="AY55" s="11"/>
-      <c r="AZ55" s="11"/>
-      <c r="BA55" s="11"/>
-      <c r="BB55" s="11"/>
-      <c r="BC55" s="11"/>
-      <c r="BD55" s="11"/>
-      <c r="BE55" s="11"/>
-      <c r="BF55" s="10" t="s">
+      <c r="AY55" s="17"/>
+      <c r="AZ55" s="17"/>
+      <c r="BA55" s="17"/>
+      <c r="BB55" s="17"/>
+      <c r="BC55" s="17"/>
+      <c r="BD55" s="17"/>
+      <c r="BE55" s="17"/>
+      <c r="BF55" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="BG55" s="10"/>
-      <c r="BH55" s="10"/>
-      <c r="BI55" s="10"/>
-      <c r="BJ55" s="10"/>
-      <c r="BK55" s="10"/>
-      <c r="BL55" s="10"/>
-      <c r="BM55" s="10"/>
+      <c r="BG55" s="18"/>
+      <c r="BH55" s="18"/>
+      <c r="BI55" s="18"/>
+      <c r="BJ55" s="18"/>
+      <c r="BK55" s="18"/>
+      <c r="BL55" s="18"/>
+      <c r="BM55" s="18"/>
+    </row>
+    <row r="56" spans="2:65" x14ac:dyDescent="0.25">
+      <c r="B56">
+        <v>24</v>
+      </c>
+      <c r="J56">
+        <v>25</v>
+      </c>
+      <c r="R56">
+        <v>26</v>
+      </c>
+      <c r="Z56">
+        <v>27</v>
+      </c>
+      <c r="AH56">
+        <v>28</v>
+      </c>
+      <c r="AP56">
+        <v>29</v>
+      </c>
+      <c r="AX56">
+        <v>30</v>
+      </c>
+      <c r="BF56">
+        <v>31</v>
+      </c>
     </row>
     <row r="57" spans="2:65" x14ac:dyDescent="0.25">
-      <c r="B57" s="17"/>
-      <c r="C57" s="17"/>
-      <c r="D57" s="17"/>
-      <c r="E57" s="17"/>
-      <c r="F57" s="17"/>
-      <c r="G57" s="17"/>
-      <c r="H57" s="17"/>
-      <c r="I57" s="17"/>
-      <c r="J57" s="16"/>
-      <c r="K57" s="16"/>
-      <c r="L57" s="16"/>
-      <c r="M57" s="16"/>
-      <c r="N57" s="16"/>
-      <c r="O57" s="16"/>
-      <c r="P57" s="16"/>
-      <c r="Q57" s="16"/>
-      <c r="R57" s="14"/>
-      <c r="S57" s="14"/>
-      <c r="T57" s="14"/>
-      <c r="U57" s="14"/>
-      <c r="V57" s="14"/>
-      <c r="W57" s="14"/>
-      <c r="X57" s="14"/>
-      <c r="Y57" s="14"/>
-      <c r="Z57" s="15"/>
-      <c r="AA57" s="15"/>
-      <c r="AB57" s="15"/>
-      <c r="AC57" s="15"/>
-      <c r="AD57" s="15"/>
-      <c r="AE57" s="15"/>
-      <c r="AF57" s="15"/>
-      <c r="AG57" s="15"/>
-      <c r="AH57" s="12"/>
-      <c r="AI57" s="12"/>
-      <c r="AJ57" s="12"/>
-      <c r="AK57" s="12"/>
-      <c r="AL57" s="12"/>
-      <c r="AM57" s="12"/>
-      <c r="AN57" s="12"/>
-      <c r="AO57" s="12"/>
-      <c r="AP57" s="13"/>
-      <c r="AQ57" s="13"/>
-      <c r="AR57" s="13"/>
-      <c r="AS57" s="13"/>
-      <c r="AT57" s="13"/>
-      <c r="AU57" s="13"/>
-      <c r="AV57" s="13"/>
-      <c r="AW57" s="13"/>
-      <c r="AX57" s="11"/>
-      <c r="AY57" s="11"/>
-      <c r="AZ57" s="11"/>
-      <c r="BA57" s="11"/>
-      <c r="BB57" s="11"/>
-      <c r="BC57" s="11"/>
-      <c r="BD57" s="11"/>
-      <c r="BE57" s="11"/>
-      <c r="BF57" s="10"/>
-      <c r="BG57" s="10"/>
-      <c r="BH57" s="10"/>
-      <c r="BI57" s="10"/>
-      <c r="BJ57" s="10"/>
-      <c r="BK57" s="10"/>
-      <c r="BL57" s="10"/>
-      <c r="BM57" s="10"/>
+      <c r="B57" s="11"/>
+      <c r="C57" s="11"/>
+      <c r="D57" s="11"/>
+      <c r="E57" s="11"/>
+      <c r="F57" s="11"/>
+      <c r="G57" s="11"/>
+      <c r="H57" s="11"/>
+      <c r="I57" s="11"/>
+      <c r="J57" s="12"/>
+      <c r="K57" s="12"/>
+      <c r="L57" s="12"/>
+      <c r="M57" s="12"/>
+      <c r="N57" s="12"/>
+      <c r="O57" s="12"/>
+      <c r="P57" s="12"/>
+      <c r="Q57" s="12"/>
+      <c r="R57" s="13"/>
+      <c r="S57" s="13"/>
+      <c r="T57" s="13"/>
+      <c r="U57" s="13"/>
+      <c r="V57" s="13"/>
+      <c r="W57" s="13"/>
+      <c r="X57" s="13"/>
+      <c r="Y57" s="13"/>
+      <c r="Z57" s="14"/>
+      <c r="AA57" s="14"/>
+      <c r="AB57" s="14"/>
+      <c r="AC57" s="14"/>
+      <c r="AD57" s="14"/>
+      <c r="AE57" s="14"/>
+      <c r="AF57" s="14"/>
+      <c r="AG57" s="14"/>
+      <c r="AH57" s="15"/>
+      <c r="AI57" s="15"/>
+      <c r="AJ57" s="15"/>
+      <c r="AK57" s="15"/>
+      <c r="AL57" s="15"/>
+      <c r="AM57" s="15"/>
+      <c r="AN57" s="15"/>
+      <c r="AO57" s="15"/>
+      <c r="AP57" s="16"/>
+      <c r="AQ57" s="16"/>
+      <c r="AR57" s="16"/>
+      <c r="AS57" s="16"/>
+      <c r="AT57" s="16"/>
+      <c r="AU57" s="16"/>
+      <c r="AV57" s="16"/>
+      <c r="AW57" s="16"/>
+      <c r="AX57" s="17"/>
+      <c r="AY57" s="17"/>
+      <c r="AZ57" s="17"/>
+      <c r="BA57" s="17"/>
+      <c r="BB57" s="17"/>
+      <c r="BC57" s="17"/>
+      <c r="BD57" s="17"/>
+      <c r="BE57" s="17"/>
+      <c r="BF57" s="18"/>
+      <c r="BG57" s="18"/>
+      <c r="BH57" s="18"/>
+      <c r="BI57" s="18"/>
+      <c r="BJ57" s="18"/>
+      <c r="BK57" s="18"/>
+      <c r="BL57" s="18"/>
+      <c r="BM57" s="18"/>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>99</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="71">
-    <mergeCell ref="X6:AE6"/>
-    <mergeCell ref="BT6:CA6"/>
-    <mergeCell ref="BL6:BS6"/>
-    <mergeCell ref="BD6:BK6"/>
-    <mergeCell ref="AV6:BC6"/>
-    <mergeCell ref="AN6:AU6"/>
-    <mergeCell ref="AF6:AM6"/>
-    <mergeCell ref="B41:I41"/>
-    <mergeCell ref="J43:Q43"/>
-    <mergeCell ref="J41:Q41"/>
-    <mergeCell ref="J45:Q45"/>
-    <mergeCell ref="J47:Q47"/>
-    <mergeCell ref="J51:Q51"/>
-    <mergeCell ref="J53:Q53"/>
-    <mergeCell ref="J55:Q55"/>
-    <mergeCell ref="J57:Q57"/>
-    <mergeCell ref="B43:I43"/>
-    <mergeCell ref="B45:I45"/>
-    <mergeCell ref="B47:I47"/>
-    <mergeCell ref="B51:I51"/>
-    <mergeCell ref="B53:I53"/>
-    <mergeCell ref="B55:I55"/>
-    <mergeCell ref="B57:I57"/>
+    <mergeCell ref="BF47:BM47"/>
+    <mergeCell ref="BF51:BM51"/>
+    <mergeCell ref="BF53:BM53"/>
+    <mergeCell ref="BF55:BM55"/>
+    <mergeCell ref="BF57:BM57"/>
+    <mergeCell ref="AX45:BE45"/>
+    <mergeCell ref="AX43:BE43"/>
+    <mergeCell ref="AX41:BE41"/>
+    <mergeCell ref="BF41:BM41"/>
+    <mergeCell ref="BF43:BM43"/>
+    <mergeCell ref="BF45:BM45"/>
+    <mergeCell ref="AX57:BE57"/>
+    <mergeCell ref="AX55:BE55"/>
+    <mergeCell ref="AX53:BE53"/>
+    <mergeCell ref="AX51:BE51"/>
+    <mergeCell ref="AX47:BE47"/>
+    <mergeCell ref="AH53:AO53"/>
+    <mergeCell ref="AH55:AO55"/>
+    <mergeCell ref="AH57:AO57"/>
+    <mergeCell ref="AP41:AW41"/>
+    <mergeCell ref="AP43:AW43"/>
+    <mergeCell ref="AP45:AW45"/>
+    <mergeCell ref="AP47:AW47"/>
+    <mergeCell ref="AP51:AW51"/>
+    <mergeCell ref="AP53:AW53"/>
+    <mergeCell ref="AP55:AW55"/>
+    <mergeCell ref="AP57:AW57"/>
+    <mergeCell ref="AH41:AO41"/>
+    <mergeCell ref="AH43:AO43"/>
+    <mergeCell ref="AH45:AO45"/>
+    <mergeCell ref="AH47:AO47"/>
+    <mergeCell ref="AH51:AO51"/>
     <mergeCell ref="R53:Y53"/>
     <mergeCell ref="R55:Y55"/>
     <mergeCell ref="R57:Y57"/>
@@ -2882,38 +2936,29 @@
     <mergeCell ref="R45:Y45"/>
     <mergeCell ref="R47:Y47"/>
     <mergeCell ref="R51:Y51"/>
-    <mergeCell ref="AH53:AO53"/>
-    <mergeCell ref="AH55:AO55"/>
-    <mergeCell ref="AH57:AO57"/>
-    <mergeCell ref="AP41:AW41"/>
-    <mergeCell ref="AP43:AW43"/>
-    <mergeCell ref="AP45:AW45"/>
-    <mergeCell ref="AP47:AW47"/>
-    <mergeCell ref="AP51:AW51"/>
-    <mergeCell ref="AP53:AW53"/>
-    <mergeCell ref="AP55:AW55"/>
-    <mergeCell ref="AP57:AW57"/>
-    <mergeCell ref="AH41:AO41"/>
-    <mergeCell ref="AH43:AO43"/>
-    <mergeCell ref="AH45:AO45"/>
-    <mergeCell ref="AH47:AO47"/>
-    <mergeCell ref="AH51:AO51"/>
-    <mergeCell ref="AX57:BE57"/>
-    <mergeCell ref="AX55:BE55"/>
-    <mergeCell ref="AX53:BE53"/>
-    <mergeCell ref="AX51:BE51"/>
-    <mergeCell ref="AX47:BE47"/>
-    <mergeCell ref="AX45:BE45"/>
-    <mergeCell ref="AX43:BE43"/>
-    <mergeCell ref="AX41:BE41"/>
-    <mergeCell ref="BF41:BM41"/>
-    <mergeCell ref="BF43:BM43"/>
-    <mergeCell ref="BF45:BM45"/>
-    <mergeCell ref="BF47:BM47"/>
-    <mergeCell ref="BF51:BM51"/>
-    <mergeCell ref="BF53:BM53"/>
-    <mergeCell ref="BF55:BM55"/>
-    <mergeCell ref="BF57:BM57"/>
+    <mergeCell ref="J51:Q51"/>
+    <mergeCell ref="J53:Q53"/>
+    <mergeCell ref="J55:Q55"/>
+    <mergeCell ref="J57:Q57"/>
+    <mergeCell ref="B43:I43"/>
+    <mergeCell ref="B45:I45"/>
+    <mergeCell ref="B47:I47"/>
+    <mergeCell ref="B51:I51"/>
+    <mergeCell ref="B53:I53"/>
+    <mergeCell ref="B55:I55"/>
+    <mergeCell ref="B57:I57"/>
+    <mergeCell ref="B41:I41"/>
+    <mergeCell ref="J43:Q43"/>
+    <mergeCell ref="J41:Q41"/>
+    <mergeCell ref="J45:Q45"/>
+    <mergeCell ref="J47:Q47"/>
+    <mergeCell ref="X6:AE6"/>
+    <mergeCell ref="BT6:CA6"/>
+    <mergeCell ref="BL6:BS6"/>
+    <mergeCell ref="BD6:BK6"/>
+    <mergeCell ref="AV6:BC6"/>
+    <mergeCell ref="AN6:AU6"/>
+    <mergeCell ref="AF6:AM6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>